<commit_message>
MELHORADA Tarefa 1 - Aula 2
</commit_message>
<xml_diff>
--- a/Aula 1/3515 L01 Sched 2020.xlsx
+++ b/Aula 1/3515 L01 Sched 2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr codeName="EstaPasta_de_trabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prof. Marco Mesquita\Dropbox\PRO3515\2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thale\Documents\Faculdade\PRO3515 - Algoritmos de Otimização para Problemas de Programação da Produção\Aula 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB753950-45D8-43F7-9E39-D3E624E5A005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C662B2-E8C5-4FCC-9928-4884AF444022}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1095" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M1" sheetId="30" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="52">
   <si>
     <t>#</t>
   </si>
@@ -227,7 +227,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -335,6 +335,10 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -359,7 +363,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -439,6 +443,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -451,7 +456,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1575,7 +1585,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1651,7 +1661,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A</c:v>
+                  <c:v>D</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1708,7 +1718,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1767,7 +1777,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B</c:v>
+                  <c:v>E</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1824,7 +1834,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1883,7 +1893,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C</c:v>
+                  <c:v>A</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1940,7 +1950,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1999,7 +2009,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>D</c:v>
+                  <c:v>C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2056,7 +2066,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2115,7 +2125,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>E</c:v>
+                  <c:v>B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2172,7 +2182,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2297,7 +2307,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2985,7 +2995,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3673,7 +3683,7 @@
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4361,7 +4371,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5634,7 +5644,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6904,7 +6914,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8183,7 +8193,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8986,7 +8996,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -9788,7 +9798,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -10071,7 +10081,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10110,7 +10120,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10199,7 +10209,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10337,7 +10347,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11053,7 +11063,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -11326,7 +11336,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11365,7 +11375,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11454,7 +11464,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12268,7 +12278,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -12551,7 +12561,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12679,7 +12689,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12807,7 +12817,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13607,8 +13617,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2120709" cy="1817485"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CaixaDeTexto 3">
@@ -13980,7 +13990,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -14007,7 +14017,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -14047,7 +14057,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -14091,7 +14101,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CaixaDeTexto 3">
@@ -15243,10 +15253,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="M1_Tab0" displayName="M1_Tab0" ref="B14:E19" totalsRowShown="0" headerRowDxfId="115">
-  <autoFilter ref="B14:E19" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B15:E19">
-    <sortCondition ref="C14:C19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="M1_Tab0" displayName="M1_Tab0" ref="B14:E20" totalsRowShown="0" headerRowDxfId="115">
+  <autoFilter ref="B14:E20" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B15:E20">
+    <sortCondition ref="B14:B20"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#"/>
@@ -15432,8 +15442,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="M1_Tab1" displayName="M1_Tab1" ref="G14:I19" totalsRowShown="0" headerRowDxfId="114">
-  <autoFilter ref="G14:I19" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="M1_Tab1" displayName="M1_Tab1" ref="G14:I20" totalsRowShown="0" headerRowDxfId="114">
+  <autoFilter ref="G14:I20" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Job">
       <calculatedColumnFormula>C15</calculatedColumnFormula>
@@ -15632,8 +15642,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="M1_Tab2" displayName="M1_Tab2" ref="K14:O19" totalsRowShown="0" headerRowDxfId="113">
-  <autoFilter ref="K14:O19" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="M1_Tab2" displayName="M1_Tab2" ref="K14:O20" totalsRowShown="0" headerRowDxfId="113">
+  <autoFilter ref="K14:O20" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K17:O21">
     <sortCondition ref="K15:K20"/>
   </sortState>
@@ -15857,8 +15867,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="M1_Tab4" displayName="M1_Tab4" ref="T14:V19" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
-  <autoFilter ref="T14:V19" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="M1_Tab4" displayName="M1_Tab4" ref="T14:V20" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
+  <autoFilter ref="T14:V20" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Job" dataDxfId="110">
       <calculatedColumnFormula>G15</calculatedColumnFormula>
@@ -16361,18 +16371,18 @@
   <dimension ref="A1:AF27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="16" width="5.6640625" style="13" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" style="13" customWidth="1"/>
-    <col min="18" max="26" width="5.6640625" style="13" customWidth="1"/>
-    <col min="27" max="16384" width="8.88671875" style="13"/>
+    <col min="1" max="16" width="5.6328125" style="13" customWidth="1"/>
+    <col min="17" max="17" width="20.6328125" style="13" customWidth="1"/>
+    <col min="18" max="26" width="5.6328125" style="13" customWidth="1"/>
+    <col min="27" max="16384" width="8.90625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="12" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:32" s="12" customFormat="1" ht="26">
       <c r="A1" s="10" t="s">
         <v>26</v>
       </c>
@@ -16395,7 +16405,7 @@
       <c r="R1" s="10"/>
       <c r="S1" s="10"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32">
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -16414,12 +16424,12 @@
       <c r="Q2" s="14"/>
       <c r="R2" s="14"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32">
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32">
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -16433,7 +16443,7 @@
       <c r="Z4" s="15"/>
       <c r="AA4" s="15"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -16447,7 +16457,7 @@
       <c r="Z5" s="15"/>
       <c r="AA5" s="15"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32">
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -16461,28 +16471,28 @@
       <c r="Z6" s="15"/>
       <c r="AA6" s="15"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32">
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32">
       <c r="T10" s="15"/>
       <c r="U10" s="15"/>
       <c r="V10" s="15"/>
@@ -16497,7 +16507,7 @@
       <c r="AE10" s="15"/>
       <c r="AF10" s="15"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32">
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
@@ -16513,7 +16523,7 @@
       <c r="AE11" s="15"/>
       <c r="AF11" s="15"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32">
       <c r="B12" s="16" t="s">
         <v>24</v>
       </c>
@@ -16523,11 +16533,11 @@
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
       <c r="S12" s="15"/>
-      <c r="T12" s="43" t="s">
+      <c r="T12" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="U12" s="43"/>
-      <c r="V12" s="43"/>
+      <c r="U12" s="44"/>
+      <c r="V12" s="44"/>
       <c r="W12" s="15"/>
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
@@ -16536,7 +16546,7 @@
       <c r="AB12" s="15"/>
       <c r="AC12" s="15"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32">
       <c r="B13" s="15"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -16561,7 +16571,7 @@
       <c r="AB13" s="15"/>
       <c r="AC13" s="15"/>
     </row>
-    <row r="14" spans="1:32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" customFormat="1" ht="13">
       <c r="B14" s="41" t="s">
         <v>0</v>
       </c>
@@ -16614,21 +16624,23 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B15" s="15"/>
+    <row r="15" spans="1:32">
+      <c r="B15" s="15">
+        <v>1</v>
+      </c>
       <c r="C15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="15">
         <v>4</v>
       </c>
-      <c r="D15" s="15">
-        <v>3</v>
-      </c>
       <c r="E15" s="15">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15" t="str">
         <f>C15</f>
-        <v>A</v>
+        <v>D</v>
       </c>
       <c r="H15" s="15">
         <f>IF(ISNUMBER(I14),I14,0)</f>
@@ -16636,24 +16648,24 @@
       </c>
       <c r="I15" s="15">
         <f>H15+D15</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J15" s="15"/>
       <c r="K15" s="15" t="str">
         <f>G15</f>
-        <v>A</v>
+        <v>D</v>
       </c>
       <c r="L15" s="15">
         <f>I15</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M15" s="15">
         <f>E15</f>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="N15" s="15">
         <f>L15-M15</f>
-        <v>-4</v>
+        <v>-14</v>
       </c>
       <c r="O15" s="15">
         <f>MAX(0,N15)</f>
@@ -16664,11 +16676,11 @@
       </c>
       <c r="R15" s="9">
         <f>MAX(M1_Tab2[C])</f>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="T15" s="17" t="str">
         <f>G15</f>
-        <v>A</v>
+        <v>D</v>
       </c>
       <c r="U15" s="35">
         <f>H15</f>
@@ -16676,51 +16688,53 @@
       </c>
       <c r="V15" s="35">
         <f>I15-H15</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W15" s="15"/>
       <c r="X15" s="15"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B16" s="15"/>
+    <row r="16" spans="1:32">
+      <c r="B16" s="15">
+        <v>2</v>
+      </c>
       <c r="C16" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="15">
         <v>5</v>
       </c>
-      <c r="D16" s="15">
-        <v>4</v>
-      </c>
       <c r="E16" s="15">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15" t="str">
         <f>C16</f>
-        <v>B</v>
+        <v>E</v>
       </c>
       <c r="H16" s="15">
         <f>IF(ISNUMBER(I15),I15,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I16" s="15">
         <f>H16+D16</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15" t="str">
         <f>G16</f>
-        <v>B</v>
+        <v>E</v>
       </c>
       <c r="L16" s="15">
         <f>I16</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M16" s="15">
         <f>E16</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="N16" s="15">
         <f>L16-M16</f>
-        <v>-1</v>
+        <v>-8</v>
       </c>
       <c r="O16" s="15">
         <f>MAX(0,N16)</f>
@@ -16731,11 +16745,11 @@
       </c>
       <c r="R16" s="9">
         <f>AVERAGE(M1_Tab2[C])</f>
-        <v>10</v>
+        <v>14.5</v>
       </c>
       <c r="T16" s="17" t="str">
         <f>G16</f>
-        <v>B</v>
+        <v>E</v>
       </c>
       <c r="U16" s="35">
         <f t="shared" ref="U16:U19" si="0">H16-I15</f>
@@ -16743,51 +16757,53 @@
       </c>
       <c r="V16" s="35">
         <f t="shared" ref="V16:V19" si="1">I16-H16</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W16" s="15"/>
       <c r="X16" s="15"/>
     </row>
-    <row r="17" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B17" s="15"/>
+    <row r="17" spans="2:32">
+      <c r="B17" s="15">
+        <v>3</v>
+      </c>
       <c r="C17" s="15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" s="15">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E17" s="15">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15" t="str">
         <f>C17</f>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="H17" s="15">
         <f>IF(ISNUMBER(I16),I16,0)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I17" s="15">
         <f>H17+D17</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15" t="str">
         <f>G17</f>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="L17" s="15">
         <f>I17</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M17" s="15">
         <f>E17</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="N17" s="15">
         <f>L17-M17</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="O17" s="15">
         <f>MAX(0,N17)</f>
@@ -16798,11 +16814,11 @@
       </c>
       <c r="R17" s="9">
         <f>SUM(M1_Tab2[T])</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T17" s="17" t="str">
         <f>G17</f>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="U17" s="35">
         <f t="shared" si="0"/>
@@ -16810,66 +16826,68 @@
       </c>
       <c r="V17" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="W17" s="15"/>
       <c r="X17" s="15"/>
     </row>
-    <row r="18" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B18" s="15"/>
+    <row r="18" spans="2:32">
+      <c r="B18" s="15">
+        <v>4</v>
+      </c>
       <c r="C18" s="15" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D18" s="15">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E18" s="15">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="15" t="str">
         <f>C18</f>
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="H18" s="15">
         <f>IF(ISNUMBER(I17),I17,0)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I18" s="15">
         <f>H18+D18</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15" t="str">
         <f>G18</f>
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="L18" s="15">
         <f>I18</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M18" s="15">
         <f>E18</f>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N18" s="15">
         <f>L18-M18</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="O18" s="15">
         <f>MAX(0,N18)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="s">
         <v>21</v>
       </c>
       <c r="R18" s="9">
         <f>MAX(M1_Tab2[T])</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="T18" s="17" t="str">
         <f>G18</f>
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="U18" s="35">
         <f t="shared" si="0"/>
@@ -16877,66 +16895,68 @@
       </c>
       <c r="V18" s="35">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
     </row>
-    <row r="19" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B19" s="15"/>
+    <row r="19" spans="2:32">
+      <c r="B19" s="15">
+        <v>5</v>
+      </c>
       <c r="C19" s="15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D19" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="15">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15" t="str">
         <f>C19</f>
-        <v>E</v>
+        <v>B</v>
       </c>
       <c r="H19" s="15">
         <f>IF(ISNUMBER(I18),I18,0)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I19" s="15">
         <f>H19+D19</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J19" s="15"/>
       <c r="K19" s="15" t="str">
         <f>G19</f>
-        <v>E</v>
+        <v>B</v>
       </c>
       <c r="L19" s="15">
         <f>I19</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="M19" s="15">
         <f>E19</f>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="N19" s="15">
         <f>L19-M19</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="O19" s="15">
         <f>MAX(0,N19)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="Q19" t="s">
         <v>22</v>
       </c>
       <c r="R19" s="25">
         <f>COUNTIF(M1_Tab2[T],"&gt;0")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T19" s="17" t="str">
         <f>G19</f>
-        <v>E</v>
+        <v>B</v>
       </c>
       <c r="U19" s="35">
         <f t="shared" si="0"/>
@@ -16944,36 +16964,77 @@
       </c>
       <c r="V19" s="35">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W19" s="15"/>
       <c r="X19" s="15"/>
     </row>
-    <row r="20" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+    <row r="20" spans="2:32">
+      <c r="B20" s="18">
+        <v>6</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="18">
+        <v>1</v>
+      </c>
+      <c r="E20" s="18">
+        <v>21</v>
+      </c>
       <c r="F20" s="15"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="G20" s="18" t="str">
+        <f>C20</f>
+        <v>F</v>
+      </c>
+      <c r="H20" s="18">
+        <f>IF(ISNUMBER(I19),I19,0)</f>
+        <v>20</v>
+      </c>
+      <c r="I20" s="18">
+        <f>H20+D20</f>
+        <v>21</v>
+      </c>
       <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
+      <c r="K20" s="18" t="str">
+        <f>G20</f>
+        <v>F</v>
+      </c>
+      <c r="L20" s="18">
+        <f>I20</f>
+        <v>21</v>
+      </c>
+      <c r="M20" s="18">
+        <f>E20</f>
+        <v>21</v>
+      </c>
+      <c r="N20" s="18">
+        <f>L20-M20</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="18">
+        <f>MAX(0,N20)</f>
+        <v>0</v>
+      </c>
       <c r="P20" s="15"/>
       <c r="Q20" s="20"/>
       <c r="R20" s="20"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
+      <c r="T20" s="48" t="str">
+        <f>G20</f>
+        <v>F</v>
+      </c>
+      <c r="U20" s="49">
+        <f>H20</f>
+        <v>20</v>
+      </c>
+      <c r="V20" s="49">
+        <f>I20-H20</f>
+        <v>1</v>
+      </c>
       <c r="W20" s="15"/>
       <c r="X20" s="15"/>
     </row>
-    <row r="21" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:32">
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -16997,7 +17058,7 @@
       <c r="W21" s="15"/>
       <c r="X21" s="15"/>
     </row>
-    <row r="22" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:32">
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -17026,7 +17087,7 @@
       <c r="AB22" s="15"/>
       <c r="AC22" s="15"/>
     </row>
-    <row r="23" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:32">
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -17055,7 +17116,7 @@
       <c r="AB23" s="15"/>
       <c r="AC23" s="15"/>
     </row>
-    <row r="24" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:32">
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
@@ -17084,7 +17145,7 @@
       <c r="AB24" s="15"/>
       <c r="AC24" s="15"/>
     </row>
-    <row r="25" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:32">
       <c r="T25" s="15"/>
       <c r="U25" s="15"/>
       <c r="V25" s="15"/>
@@ -17096,7 +17157,7 @@
       <c r="AB25" s="15"/>
       <c r="AC25" s="15"/>
     </row>
-    <row r="26" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:32">
       <c r="T26" s="15"/>
       <c r="U26" s="15"/>
       <c r="V26" s="15"/>
@@ -17111,7 +17172,7 @@
       <c r="AE26" s="15"/>
       <c r="AF26" s="15"/>
     </row>
-    <row r="27" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:32">
       <c r="T27" s="15"/>
       <c r="U27" s="15"/>
       <c r="V27" s="15"/>
@@ -17161,15 +17222,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="30" width="5.6640625" style="13" customWidth="1"/>
-    <col min="31" max="31" width="20.6640625" style="13" customWidth="1"/>
-    <col min="32" max="44" width="5.6640625" style="13" customWidth="1"/>
-    <col min="45" max="16384" width="8.88671875" style="13"/>
+    <col min="1" max="30" width="5.6328125" style="13" customWidth="1"/>
+    <col min="31" max="31" width="20.6328125" style="13" customWidth="1"/>
+    <col min="32" max="44" width="5.6328125" style="13" customWidth="1"/>
+    <col min="45" max="16384" width="8.90625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="12" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:50" s="12" customFormat="1" ht="26">
       <c r="A1" s="10" t="s">
         <v>28</v>
       </c>
@@ -17197,7 +17258,7 @@
       <c r="W1" s="10"/>
       <c r="X1" s="10"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50">
       <c r="Z3"/>
       <c r="AA3"/>
       <c r="AB3"/>
@@ -17210,7 +17271,7 @@
       <c r="AI3"/>
       <c r="AJ3"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50">
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -17232,7 +17293,7 @@
       <c r="AT4" s="15"/>
       <c r="AU4" s="15"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -17254,7 +17315,7 @@
       <c r="AT5" s="15"/>
       <c r="AU5" s="15"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50">
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -17276,7 +17337,7 @@
       <c r="AT6" s="15"/>
       <c r="AU6" s="15"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -17290,7 +17351,7 @@
       <c r="AG7" s="9"/>
       <c r="AJ7"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50">
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -17304,7 +17365,7 @@
       <c r="AG8" s="9"/>
       <c r="AJ8"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -17318,7 +17379,7 @@
       <c r="AG9" s="25"/>
       <c r="AJ9"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50">
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -17337,7 +17398,7 @@
       <c r="AP10" s="15"/>
       <c r="AQ10" s="15"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:50">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -17366,7 +17427,7 @@
       <c r="AW11" s="15"/>
       <c r="AX11" s="15"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:50">
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -17388,7 +17449,7 @@
       <c r="AW12" s="15"/>
       <c r="AX12" s="15"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:50">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -17410,7 +17471,7 @@
       <c r="AW13" s="15"/>
       <c r="AX13" s="15"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50">
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -17425,7 +17486,7 @@
       <c r="AP14" s="15"/>
       <c r="AQ14" s="15"/>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -17440,7 +17501,7 @@
       <c r="AP15" s="15"/>
       <c r="AQ15" s="15"/>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:50">
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
@@ -17462,7 +17523,7 @@
       <c r="AP16" s="15"/>
       <c r="AQ16" s="15"/>
     </row>
-    <row r="17" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:50">
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -17486,7 +17547,7 @@
       <c r="AP17" s="15"/>
       <c r="AQ17" s="15"/>
     </row>
-    <row r="18" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:50">
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -17517,7 +17578,7 @@
       <c r="AW18" s="15"/>
       <c r="AX18" s="15"/>
     </row>
-    <row r="19" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:50">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -17548,7 +17609,7 @@
       <c r="AW19" s="15"/>
       <c r="AX19" s="15"/>
     </row>
-    <row r="20" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:50">
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -17579,7 +17640,7 @@
       <c r="AW20" s="15"/>
       <c r="AX20" s="15"/>
     </row>
-    <row r="21" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:50">
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
@@ -17603,7 +17664,7 @@
       <c r="AP21" s="15"/>
       <c r="AQ21" s="15"/>
     </row>
-    <row r="22" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:50">
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
@@ -17627,7 +17688,7 @@
       <c r="AP22" s="15"/>
       <c r="AQ22" s="15"/>
     </row>
-    <row r="23" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:50">
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
@@ -17651,7 +17712,7 @@
       <c r="AP23" s="15"/>
       <c r="AQ23" s="15"/>
     </row>
-    <row r="24" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:50">
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
@@ -17675,7 +17736,7 @@
       <c r="AP24" s="15"/>
       <c r="AQ24" s="15"/>
     </row>
-    <row r="25" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:50">
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
@@ -17699,55 +17760,55 @@
       <c r="AP25" s="15"/>
       <c r="AQ25" s="15"/>
     </row>
-    <row r="26" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:50">
       <c r="B26" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="44" t="s">
+      <c r="I26" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="44"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
       <c r="M26" s="21"/>
-      <c r="N26" s="44" t="s">
+      <c r="N26" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="O26" s="44"/>
-      <c r="P26" s="44"/>
-      <c r="Q26" s="44"/>
+      <c r="O26" s="45"/>
+      <c r="P26" s="45"/>
+      <c r="Q26" s="45"/>
       <c r="R26" s="21"/>
-      <c r="S26" s="44" t="s">
+      <c r="S26" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="T26" s="44"/>
-      <c r="U26" s="44"/>
-      <c r="V26" s="44"/>
+      <c r="T26" s="45"/>
+      <c r="U26" s="45"/>
+      <c r="V26" s="45"/>
       <c r="W26" s="21"/>
       <c r="X26" s="21"/>
       <c r="Y26" s="21"/>
-      <c r="AH26" s="43" t="s">
+      <c r="AH26" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="AI26" s="43"/>
-      <c r="AJ26" s="43"/>
+      <c r="AI26" s="44"/>
+      <c r="AJ26" s="44"/>
       <c r="AK26" s="15"/>
-      <c r="AL26" s="43" t="s">
+      <c r="AL26" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="AM26" s="43"/>
-      <c r="AN26" s="43"/>
+      <c r="AM26" s="44"/>
+      <c r="AN26" s="44"/>
       <c r="AO26" s="15"/>
-      <c r="AP26" s="43" t="s">
+      <c r="AP26" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AQ26" s="43"/>
-      <c r="AR26" s="43"/>
+      <c r="AQ26" s="44"/>
+      <c r="AR26" s="44"/>
     </row>
-    <row r="27" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:50">
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
       <c r="D27" s="17"/>
@@ -17777,7 +17838,7 @@
       <c r="AQ27" s="15"/>
       <c r="AR27" s="15"/>
     </row>
-    <row r="28" spans="2:50" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:50" customFormat="1" ht="13">
       <c r="B28" s="41" t="s">
         <v>29</v>
       </c>
@@ -17884,7 +17945,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:50">
       <c r="B29" s="13">
         <v>1</v>
       </c>
@@ -17892,7 +17953,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="15">
-        <f>B29*100+C29</f>
+        <f t="shared" ref="D29:D38" si="0">B29*100+C29</f>
         <v>101</v>
       </c>
       <c r="E29" s="15" t="s">
@@ -17954,7 +18015,7 @@
       </c>
       <c r="W29" s="15"/>
       <c r="X29" s="15">
-        <f t="shared" ref="X29:X38" si="0">D29</f>
+        <f t="shared" ref="X29:X38" si="1">D29</f>
         <v>101</v>
       </c>
       <c r="Y29" s="15" t="str">
@@ -17966,15 +18027,15 @@
         <v>4</v>
       </c>
       <c r="AA29" s="15">
-        <f t="shared" ref="AA29:AA38" si="1">G29</f>
+        <f t="shared" ref="AA29:AA38" si="2">G29</f>
         <v>20</v>
       </c>
       <c r="AB29" s="15">
-        <f t="shared" ref="AB29:AB38" ca="1" si="2">Z29-AA29</f>
+        <f t="shared" ref="AB29:AB38" ca="1" si="3">Z29-AA29</f>
         <v>-16</v>
       </c>
       <c r="AC29" s="15">
-        <f t="shared" ref="AC29:AC38" ca="1" si="3">MAX(0,AB29)</f>
+        <f t="shared" ref="AC29:AC38" ca="1" si="4">MAX(0,AB29)</f>
         <v>0</v>
       </c>
       <c r="AD29" s="15"/>
@@ -17995,11 +18056,11 @@
         <v>0</v>
       </c>
       <c r="AJ29" s="37">
-        <f t="shared" ref="AJ29:AJ38" si="4">IF(L29="","",L29-K29)</f>
+        <f t="shared" ref="AJ29:AJ38" si="5">IF(L29="","",L29-K29)</f>
         <v>4</v>
       </c>
       <c r="AL29" s="37" t="str">
-        <f t="shared" ref="AL29:AL38" si="5">IF(O29="","",O29)</f>
+        <f t="shared" ref="AL29:AL38" si="6">IF(O29="","",O29)</f>
         <v>D</v>
       </c>
       <c r="AM29" s="37">
@@ -18011,7 +18072,7 @@
         <v>12</v>
       </c>
       <c r="AP29" s="37" t="str">
-        <f t="shared" ref="AP29:AP38" si="6">IF(T29="","",T29)</f>
+        <f t="shared" ref="AP29:AP38" si="7">IF(T29="","",T29)</f>
         <v>F</v>
       </c>
       <c r="AQ29" s="37">
@@ -18019,11 +18080,11 @@
         <v>0</v>
       </c>
       <c r="AR29" s="37">
-        <f t="shared" ref="AR29:AR38" si="7">IF(V29="","",V29-U29)</f>
+        <f t="shared" ref="AR29:AR38" si="8">IF(V29="","",V29-U29)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:50">
       <c r="B30" s="13">
         <v>1</v>
       </c>
@@ -18031,7 +18092,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="15">
-        <f>B30*100+C30</f>
+        <f t="shared" si="0"/>
         <v>102</v>
       </c>
       <c r="E30" s="15" t="s">
@@ -18093,7 +18154,7 @@
       </c>
       <c r="W30" s="15"/>
       <c r="X30" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>102</v>
       </c>
       <c r="Y30" s="15" t="str">
@@ -18105,15 +18166,15 @@
         <v>6</v>
       </c>
       <c r="AA30" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="AB30" s="15">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>-14</v>
       </c>
       <c r="AC30" s="15">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AD30" s="15"/>
@@ -18126,19 +18187,19 @@
       </c>
       <c r="AG30" s="15"/>
       <c r="AH30" s="37" t="str">
-        <f t="shared" ref="AH30:AH38" si="8">IF(J30="","",J30)</f>
+        <f t="shared" ref="AH30:AH38" si="9">IF(J30="","",J30)</f>
         <v>B</v>
       </c>
       <c r="AI30" s="37">
-        <f t="shared" ref="AI30:AI38" si="9">IF(K30="","",K30-L29)</f>
+        <f t="shared" ref="AI30:AI38" si="10">IF(K30="","",K30-L29)</f>
         <v>0</v>
       </c>
       <c r="AJ30" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="AL30" s="37" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>E</v>
       </c>
       <c r="AM30" s="37">
@@ -18146,11 +18207,11 @@
         <v>0</v>
       </c>
       <c r="AN30" s="37">
-        <f t="shared" ref="AN30:AN38" si="10">IF(Q30="","",Q30-P30)</f>
+        <f t="shared" ref="AN30:AN38" si="11">IF(Q30="","",Q30-P30)</f>
         <v>15</v>
       </c>
       <c r="AP30" s="37" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>G</v>
       </c>
       <c r="AQ30" s="37">
@@ -18158,11 +18219,11 @@
         <v>0</v>
       </c>
       <c r="AR30" s="37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:50">
       <c r="B31" s="13">
         <v>1</v>
       </c>
@@ -18170,7 +18231,7 @@
         <v>3</v>
       </c>
       <c r="D31" s="15">
-        <f>B31*100+C31</f>
+        <f t="shared" si="0"/>
         <v>103</v>
       </c>
       <c r="E31" s="15" t="s">
@@ -18191,7 +18252,7 @@
         <v>C</v>
       </c>
       <c r="K31" s="15">
-        <f t="shared" ref="K31:K38" si="11">IF(J31="","",IF(ISNUMBER(L30),L30,0))</f>
+        <f t="shared" ref="K31:K38" si="12">IF(J31="","",IF(ISNUMBER(L30),L30,0))</f>
         <v>6</v>
       </c>
       <c r="L31" s="15">
@@ -18207,7 +18268,7 @@
         <v/>
       </c>
       <c r="P31" s="15" t="str">
-        <f t="shared" ref="P31:P38" si="12">IF(O31="","",IF(ISNUMBER(Q30),Q30,0))</f>
+        <f t="shared" ref="P31:P38" si="13">IF(O31="","",IF(ISNUMBER(Q30),Q30,0))</f>
         <v/>
       </c>
       <c r="Q31" s="15" t="str">
@@ -18223,7 +18284,7 @@
         <v>H</v>
       </c>
       <c r="U31" s="15">
-        <f t="shared" ref="U31:U38" si="13">IF(T31="","",IF(ISNUMBER(V30),V30,0))</f>
+        <f t="shared" ref="U31:U38" si="14">IF(T31="","",IF(ISNUMBER(V30),V30,0))</f>
         <v>6</v>
       </c>
       <c r="V31" s="15">
@@ -18232,7 +18293,7 @@
       </c>
       <c r="W31" s="15"/>
       <c r="X31" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>103</v>
       </c>
       <c r="Y31" s="15" t="str">
@@ -18244,15 +18305,15 @@
         <v>15</v>
       </c>
       <c r="AA31" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="AB31" s="15">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>-5</v>
       </c>
       <c r="AC31" s="15">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AD31" s="15"/>
@@ -18265,43 +18326,43 @@
       </c>
       <c r="AG31" s="15"/>
       <c r="AH31" s="37" t="str">
+        <f t="shared" si="9"/>
+        <v>C</v>
+      </c>
+      <c r="AI31" s="37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AJ31" s="37">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="AL31" s="37" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AM31" s="37" t="str">
+        <f t="shared" ref="AM31:AM38" si="15">IF(P31="","",P31-Q30)</f>
+        <v/>
+      </c>
+      <c r="AN31" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AP31" s="37" t="str">
+        <f t="shared" si="7"/>
+        <v>H</v>
+      </c>
+      <c r="AQ31" s="37">
+        <f t="shared" ref="AQ31:AQ38" si="16">IF(U31="","",U31-V30)</f>
+        <v>0</v>
+      </c>
+      <c r="AR31" s="37">
         <f t="shared" si="8"/>
-        <v>C</v>
-      </c>
-      <c r="AI31" s="37">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AJ31" s="37">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="AL31" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AM31" s="37" t="str">
-        <f t="shared" ref="AM31:AM38" si="14">IF(P31="","",P31-Q30)</f>
-        <v/>
-      </c>
-      <c r="AN31" s="37" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AP31" s="37" t="str">
-        <f t="shared" si="6"/>
-        <v>H</v>
-      </c>
-      <c r="AQ31" s="37">
-        <f t="shared" ref="AQ31:AQ38" si="15">IF(U31="","",U31-V30)</f>
-        <v>0</v>
-      </c>
-      <c r="AR31" s="37">
-        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:50">
       <c r="B32" s="13">
         <v>2</v>
       </c>
@@ -18309,7 +18370,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="15">
-        <f>B32*100+C32</f>
+        <f t="shared" si="0"/>
         <v>201</v>
       </c>
       <c r="E32" s="15" t="s">
@@ -18330,7 +18391,7 @@
         <v/>
       </c>
       <c r="K32" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L32" s="15" t="str">
@@ -18346,7 +18407,7 @@
         <v/>
       </c>
       <c r="P32" s="15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="Q32" s="15" t="str">
@@ -18362,7 +18423,7 @@
         <v>I</v>
       </c>
       <c r="U32" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="V32" s="15">
@@ -18371,7 +18432,7 @@
       </c>
       <c r="W32" s="15"/>
       <c r="X32" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>201</v>
       </c>
       <c r="Y32" s="15" t="str">
@@ -18383,15 +18444,15 @@
         <v>12</v>
       </c>
       <c r="AA32" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="AB32" s="15">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>-8</v>
       </c>
       <c r="AC32" s="15">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AD32" s="15"/>
@@ -18404,43 +18465,43 @@
       </c>
       <c r="AG32" s="15"/>
       <c r="AH32" s="37" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="AI32" s="37" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
+      <c r="AI32" s="37" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
       <c r="AJ32" s="37" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AL32" s="37" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
+      <c r="AL32" s="37" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
       <c r="AM32" s="37" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AN32" s="37" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AP32" s="37" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>I</v>
       </c>
       <c r="AQ32" s="37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AR32" s="37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:44">
       <c r="B33" s="15">
         <v>2</v>
       </c>
@@ -18448,7 +18509,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="15">
-        <f>B33*100+C33</f>
+        <f t="shared" si="0"/>
         <v>202</v>
       </c>
       <c r="E33" s="15" t="s">
@@ -18469,7 +18530,7 @@
         <v/>
       </c>
       <c r="K33" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L33" s="15" t="str">
@@ -18485,7 +18546,7 @@
         <v/>
       </c>
       <c r="P33" s="15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="Q33" s="15" t="str">
@@ -18501,7 +18562,7 @@
         <v>J</v>
       </c>
       <c r="U33" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="V33" s="15">
@@ -18510,7 +18571,7 @@
       </c>
       <c r="W33" s="15"/>
       <c r="X33" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>202</v>
       </c>
       <c r="Y33" s="15" t="str">
@@ -18522,15 +18583,15 @@
         <v>27</v>
       </c>
       <c r="AA33" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="AB33" s="15">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>7</v>
       </c>
       <c r="AC33" s="15">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>7</v>
       </c>
       <c r="AD33" s="15"/>
@@ -18543,43 +18604,43 @@
       </c>
       <c r="AG33" s="15"/>
       <c r="AH33" s="37" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="AI33" s="37" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
+      <c r="AI33" s="37" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
       <c r="AJ33" s="37" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AL33" s="37" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
+      <c r="AL33" s="37" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
       <c r="AM33" s="37" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AN33" s="37" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AP33" s="37" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>J</v>
       </c>
       <c r="AQ33" s="37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AR33" s="37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:44">
       <c r="B34" s="15">
         <v>3</v>
       </c>
@@ -18587,7 +18648,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="15">
-        <f>B34*100+C34</f>
+        <f t="shared" si="0"/>
         <v>301</v>
       </c>
       <c r="E34" s="15" t="s">
@@ -18607,7 +18668,7 @@
         <v/>
       </c>
       <c r="K34" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L34" s="15" t="str">
@@ -18622,7 +18683,7 @@
         <v/>
       </c>
       <c r="P34" s="15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="Q34" s="15" t="str">
@@ -18637,7 +18698,7 @@
         <v/>
       </c>
       <c r="U34" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="V34" s="15" t="str">
@@ -18645,7 +18706,7 @@
         <v/>
       </c>
       <c r="X34" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>301</v>
       </c>
       <c r="Y34" s="15" t="str">
@@ -18657,15 +18718,15 @@
         <v>1</v>
       </c>
       <c r="AA34" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="AB34" s="15">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>-19</v>
       </c>
       <c r="AC34" s="15">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AD34" s="15"/>
@@ -18673,43 +18734,43 @@
       <c r="AF34" s="15"/>
       <c r="AG34" s="15"/>
       <c r="AH34" s="37" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AI34" s="37" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AJ34" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AL34" s="37" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AM34" s="37" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="AN34" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AP34" s="37" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AQ34" s="37" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="AR34" s="37" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AI34" s="37" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AJ34" s="37" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AL34" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AM34" s="37" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="AN34" s="37" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AP34" s="37" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="AQ34" s="37" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="AR34" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:44">
       <c r="B35" s="15">
         <v>3</v>
       </c>
@@ -18717,7 +18778,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="15">
-        <f>B35*100+C35</f>
+        <f t="shared" si="0"/>
         <v>302</v>
       </c>
       <c r="E35" s="15" t="s">
@@ -18737,7 +18798,7 @@
         <v/>
       </c>
       <c r="K35" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L35" s="15" t="str">
@@ -18752,7 +18813,7 @@
         <v/>
       </c>
       <c r="P35" s="15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="Q35" s="15" t="str">
@@ -18767,7 +18828,7 @@
         <v/>
       </c>
       <c r="U35" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="V35" s="15" t="str">
@@ -18775,7 +18836,7 @@
         <v/>
       </c>
       <c r="X35" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>302</v>
       </c>
       <c r="Y35" s="15" t="str">
@@ -18787,15 +18848,15 @@
         <v>6</v>
       </c>
       <c r="AA35" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="AB35" s="15">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>-14</v>
       </c>
       <c r="AC35" s="15">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AD35" s="15"/>
@@ -18803,43 +18864,43 @@
       <c r="AF35" s="15"/>
       <c r="AG35" s="15"/>
       <c r="AH35" s="37" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AI35" s="37" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AJ35" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AL35" s="37" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AM35" s="37" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="AN35" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AP35" s="37" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AQ35" s="37" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="AR35" s="37" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AI35" s="37" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AJ35" s="37" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AL35" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AM35" s="37" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="AN35" s="37" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AP35" s="37" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="AQ35" s="37" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="AR35" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:44">
       <c r="A36" s="15"/>
       <c r="B36" s="13">
         <v>3</v>
@@ -18848,7 +18909,7 @@
         <v>3</v>
       </c>
       <c r="D36" s="15">
-        <f>B36*100+C36</f>
+        <f t="shared" si="0"/>
         <v>303</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -18869,7 +18930,7 @@
         <v/>
       </c>
       <c r="K36" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L36" s="15" t="str">
@@ -18885,7 +18946,7 @@
         <v/>
       </c>
       <c r="P36" s="15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="Q36" s="15" t="str">
@@ -18900,7 +18961,7 @@
         <v/>
       </c>
       <c r="U36" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="V36" s="15" t="str">
@@ -18908,7 +18969,7 @@
         <v/>
       </c>
       <c r="X36" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>303</v>
       </c>
       <c r="Y36" s="15" t="str">
@@ -18920,15 +18981,15 @@
         <v>7</v>
       </c>
       <c r="AA36" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="AB36" s="15">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>-13</v>
       </c>
       <c r="AC36" s="15">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AD36" s="15"/>
@@ -18936,43 +18997,43 @@
       <c r="AF36" s="15"/>
       <c r="AG36" s="15"/>
       <c r="AH36" s="37" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AI36" s="37" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AJ36" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AL36" s="37" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AM36" s="37" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="AN36" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AP36" s="37" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AQ36" s="37" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="AR36" s="37" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AI36" s="37" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AJ36" s="37" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AL36" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AM36" s="37" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="AN36" s="37" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AP36" s="37" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="AQ36" s="37" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="AR36" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:44">
       <c r="A37" s="15"/>
       <c r="B37" s="13">
         <v>3</v>
@@ -18981,7 +19042,7 @@
         <v>4</v>
       </c>
       <c r="D37" s="15">
-        <f>B37*100+C37</f>
+        <f t="shared" si="0"/>
         <v>304</v>
       </c>
       <c r="E37" s="15" t="s">
@@ -19002,7 +19063,7 @@
         <v/>
       </c>
       <c r="K37" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L37" s="15" t="str">
@@ -19018,7 +19079,7 @@
         <v/>
       </c>
       <c r="P37" s="15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="Q37" s="15" t="str">
@@ -19033,7 +19094,7 @@
         <v/>
       </c>
       <c r="U37" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="V37" s="15" t="str">
@@ -19041,7 +19102,7 @@
         <v/>
       </c>
       <c r="X37" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>304</v>
       </c>
       <c r="Y37" s="15" t="str">
@@ -19053,15 +19114,15 @@
         <v>10</v>
       </c>
       <c r="AA37" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="AB37" s="15">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>-10</v>
       </c>
       <c r="AC37" s="15">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AD37" s="15"/>
@@ -19069,43 +19130,43 @@
       <c r="AF37" s="15"/>
       <c r="AG37" s="15"/>
       <c r="AH37" s="37" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AI37" s="37" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AJ37" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AL37" s="37" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AM37" s="37" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="AN37" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AP37" s="37" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AQ37" s="37" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="AR37" s="37" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AI37" s="37" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AJ37" s="37" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AL37" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AM37" s="37" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="AN37" s="37" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AP37" s="37" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="AQ37" s="37" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="AR37" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:44">
       <c r="A38" s="15"/>
       <c r="B38" s="13">
         <v>3</v>
@@ -19114,7 +19175,7 @@
         <v>5</v>
       </c>
       <c r="D38" s="15">
-        <f>B38*100+C38</f>
+        <f t="shared" si="0"/>
         <v>305</v>
       </c>
       <c r="E38" s="13" t="s">
@@ -19135,7 +19196,7 @@
         <v/>
       </c>
       <c r="K38" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L38" s="15" t="str">
@@ -19151,7 +19212,7 @@
         <v/>
       </c>
       <c r="P38" s="15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="Q38" s="15" t="str">
@@ -19166,7 +19227,7 @@
         <v/>
       </c>
       <c r="U38" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="V38" s="15" t="str">
@@ -19174,7 +19235,7 @@
         <v/>
       </c>
       <c r="X38" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>305</v>
       </c>
       <c r="Y38" s="15" t="str">
@@ -19186,15 +19247,15 @@
         <v>17</v>
       </c>
       <c r="AA38" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="AB38" s="15">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>-3</v>
       </c>
       <c r="AC38" s="15">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AD38" s="15"/>
@@ -19202,43 +19263,43 @@
       <c r="AF38" s="15"/>
       <c r="AG38" s="15"/>
       <c r="AH38" s="37" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AI38" s="37" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AJ38" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AL38" s="37" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AM38" s="37" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="AN38" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AP38" s="37" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AQ38" s="37" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="AR38" s="37" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AI38" s="37" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AJ38" s="37" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AL38" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AM38" s="37" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="AN38" s="37" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AP38" s="37" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="AQ38" s="37" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="AR38" s="37" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:44">
       <c r="A39" s="15"/>
       <c r="B39" s="33"/>
       <c r="C39" s="33"/>
@@ -19257,7 +19318,7 @@
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:44">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -19275,7 +19336,7 @@
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:44">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -19293,7 +19354,7 @@
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:44">
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -19311,7 +19372,7 @@
       <c r="Q42" s="15"/>
       <c r="R42" s="15"/>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:44">
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -19329,7 +19390,7 @@
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:44">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -19347,21 +19408,21 @@
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:44">
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:44">
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:44">
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
       <c r="F47" s="15"/>
@@ -19409,15 +19470,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="21" width="5.6640625" style="13" customWidth="1"/>
-    <col min="22" max="22" width="20.6640625" style="13" customWidth="1"/>
-    <col min="23" max="31" width="5.6640625" style="13" customWidth="1"/>
-    <col min="32" max="16384" width="8.88671875" style="13"/>
+    <col min="1" max="21" width="5.6328125" style="13" customWidth="1"/>
+    <col min="22" max="22" width="20.6328125" style="13" customWidth="1"/>
+    <col min="23" max="31" width="5.6328125" style="13" customWidth="1"/>
+    <col min="32" max="16384" width="8.90625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="12" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:33" s="12" customFormat="1" ht="26">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -19445,7 +19506,7 @@
       <c r="W1" s="10"/>
       <c r="X1" s="10"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33">
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -19459,7 +19520,7 @@
       <c r="AC3"/>
       <c r="AD3"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33">
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -19476,7 +19537,7 @@
       <c r="AF4" s="15"/>
       <c r="AG4" s="15"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -19491,7 +19552,7 @@
       <c r="AD5"/>
       <c r="AE5" s="15"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33">
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -19506,7 +19567,7 @@
       <c r="AD6"/>
       <c r="AE6" s="15"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -19520,7 +19581,7 @@
       <c r="AC7"/>
       <c r="AD7"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33">
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -19534,7 +19595,7 @@
       <c r="AC8"/>
       <c r="AD8"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -19548,7 +19609,7 @@
       <c r="AC9"/>
       <c r="AD9"/>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33">
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -19562,7 +19623,7 @@
       <c r="AC10"/>
       <c r="AD10"/>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -19578,7 +19639,7 @@
       <c r="AD11"/>
       <c r="AE11" s="15"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33">
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -19594,7 +19655,7 @@
       <c r="AD12"/>
       <c r="AE12" s="15"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -19610,36 +19671,36 @@
       <c r="AD13" s="15"/>
       <c r="AE13" s="15"/>
     </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:31">
       <c r="B18" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="44" t="s">
+      <c r="H18" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="L18" s="44" t="s">
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="L18" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="M18" s="44"/>
-      <c r="N18" s="44"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
       <c r="U18" s="15"/>
       <c r="V18" s="15"/>
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
-      <c r="Y18" s="43" t="s">
+      <c r="Y18" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="Z18" s="43"/>
-      <c r="AA18" s="43"/>
-      <c r="AC18" s="43" t="s">
+      <c r="Z18" s="44"/>
+      <c r="AA18" s="44"/>
+      <c r="AC18" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="AD18" s="43"/>
-      <c r="AE18" s="43"/>
+      <c r="AD18" s="44"/>
+      <c r="AE18" s="44"/>
     </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:31">
       <c r="B19" s="15"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -19664,7 +19725,7 @@
       <c r="AD19" s="15"/>
       <c r="AE19" s="15"/>
     </row>
-    <row r="20" spans="2:31" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:31" customFormat="1" ht="13">
       <c r="B20" s="41" t="s">
         <v>0</v>
       </c>
@@ -19738,7 +19799,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:31">
       <c r="B21" s="15"/>
       <c r="C21" s="15" t="s">
         <v>4</v>
@@ -19831,7 +19892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:31">
       <c r="B22" s="15"/>
       <c r="C22" s="15" t="s">
         <v>5</v>
@@ -19924,7 +19985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:31">
       <c r="B23" s="15"/>
       <c r="C23" s="15" t="s">
         <v>3</v>
@@ -20017,7 +20078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:31">
       <c r="B24" s="15"/>
       <c r="C24" s="15" t="s">
         <v>6</v>
@@ -20110,7 +20171,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:31">
       <c r="B25" s="15"/>
       <c r="C25" s="15" t="s">
         <v>7</v>
@@ -20203,7 +20264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:31">
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -20235,7 +20296,7 @@
       <c r="AD26" s="15"/>
       <c r="AE26" s="15"/>
     </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:31">
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -20263,7 +20324,7 @@
       <c r="AD27" s="17"/>
       <c r="AE27" s="17"/>
     </row>
-    <row r="28" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:31">
       <c r="B28" s="24"/>
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
@@ -20284,7 +20345,7 @@
       <c r="S28" s="14"/>
       <c r="T28" s="14"/>
     </row>
-    <row r="29" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:31">
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
@@ -20339,16 +20400,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="41" width="5.6640625" style="1" customWidth="1"/>
-    <col min="42" max="42" width="20.6640625" style="1" customWidth="1"/>
-    <col min="43" max="64" width="5.6640625" style="1" customWidth="1"/>
-    <col min="65" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="5.6328125" customWidth="1"/>
+    <col min="2" max="41" width="5.6328125" style="1" customWidth="1"/>
+    <col min="42" max="42" width="20.6328125" style="1" customWidth="1"/>
+    <col min="43" max="64" width="5.6328125" style="1" customWidth="1"/>
+    <col min="65" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:58" ht="26">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -20382,7 +20443,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:58">
       <c r="AI2"/>
       <c r="AJ2"/>
       <c r="AK2"/>
@@ -20402,7 +20463,7 @@
       <c r="BE2"/>
       <c r="BF2"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58">
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
@@ -20424,7 +20485,7 @@
       <c r="T3" s="40"/>
       <c r="U3" s="40"/>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:58">
       <c r="X4" s="42" t="s">
         <v>48</v>
       </c>
@@ -20445,7 +20506,7 @@
       <c r="BE4"/>
       <c r="BF4"/>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:58">
       <c r="X5" s="42" t="s">
         <v>4</v>
       </c>
@@ -20455,7 +20516,7 @@
       <c r="Z5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AD5" s="47" t="s">
+      <c r="AD5" s="43" t="s">
         <v>27</v>
       </c>
       <c r="AE5" s="32" t="s">
@@ -20484,7 +20545,7 @@
       <c r="BE5"/>
       <c r="BF5"/>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:58">
       <c r="X6" s="42" t="s">
         <v>5</v>
       </c>
@@ -20497,7 +20558,7 @@
       <c r="AA6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AD6" s="47" t="s">
+      <c r="AD6" s="43" t="s">
         <v>30</v>
       </c>
       <c r="AE6" s="32" t="s">
@@ -20523,7 +20584,7 @@
       <c r="BE6"/>
       <c r="BF6"/>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:58">
       <c r="X7" s="42" t="s">
         <v>3</v>
       </c>
@@ -20533,7 +20594,7 @@
       <c r="Z7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AD7" s="47" t="s">
+      <c r="AD7" s="43" t="s">
         <v>31</v>
       </c>
       <c r="AE7" s="32" t="s">
@@ -20562,7 +20623,7 @@
       <c r="BE7"/>
       <c r="BF7"/>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:58">
       <c r="X8" s="42" t="s">
         <v>6</v>
       </c>
@@ -20586,7 +20647,7 @@
       <c r="BE8"/>
       <c r="BF8"/>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:58">
       <c r="X9" s="42" t="s">
         <v>7</v>
       </c>
@@ -20610,7 +20671,7 @@
       <c r="BE9"/>
       <c r="BF9"/>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:58">
       <c r="AN10"/>
       <c r="AR10"/>
       <c r="AS10"/>
@@ -20625,7 +20686,7 @@
       <c r="BE10"/>
       <c r="BF10"/>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:58">
       <c r="AC11" s="32" t="s">
         <v>41</v>
       </c>
@@ -20643,8 +20704,8 @@
       <c r="BE11"/>
       <c r="BF11"/>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="AD12" s="47" t="s">
+    <row r="12" spans="1:58">
+      <c r="AD12" s="43" t="s">
         <v>27</v>
       </c>
       <c r="AE12" s="32" t="s">
@@ -20673,8 +20734,8 @@
       <c r="BE12"/>
       <c r="BF12"/>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="AD13" s="47" t="s">
+    <row r="13" spans="1:58">
+      <c r="AD13" s="43" t="s">
         <v>30</v>
       </c>
       <c r="AE13" s="32" t="s">
@@ -20700,8 +20761,8 @@
       <c r="BE13"/>
       <c r="BF13"/>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="AD14" s="47" t="s">
+    <row r="14" spans="1:58">
+      <c r="AD14" s="43" t="s">
         <v>31</v>
       </c>
       <c r="AE14" s="32" t="s">
@@ -20730,7 +20791,7 @@
       <c r="BE14"/>
       <c r="BF14"/>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:58">
       <c r="AN15"/>
       <c r="AR15"/>
       <c r="AS15"/>
@@ -20745,7 +20806,7 @@
       <c r="BE15"/>
       <c r="BF15"/>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:58">
       <c r="AN16"/>
       <c r="AR16"/>
       <c r="AS16"/>
@@ -20760,7 +20821,7 @@
       <c r="BE16"/>
       <c r="BF16"/>
     </row>
-    <row r="17" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:65">
       <c r="AN17"/>
       <c r="AR17"/>
       <c r="AS17"/>
@@ -20775,7 +20836,7 @@
       <c r="BE17"/>
       <c r="BF17"/>
     </row>
-    <row r="18" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:65">
       <c r="AC18" s="32" t="s">
         <v>42</v>
       </c>
@@ -20793,8 +20854,8 @@
       <c r="BE18"/>
       <c r="BF18"/>
     </row>
-    <row r="19" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="AD19" s="47" t="s">
+    <row r="19" spans="2:65">
+      <c r="AD19" s="43" t="s">
         <v>27</v>
       </c>
       <c r="AE19" s="32" t="s">
@@ -20823,8 +20884,8 @@
       <c r="BE19"/>
       <c r="BF19"/>
     </row>
-    <row r="20" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="AD20" s="47" t="s">
+    <row r="20" spans="2:65">
+      <c r="AD20" s="43" t="s">
         <v>30</v>
       </c>
       <c r="AE20" s="32" t="s">
@@ -20850,8 +20911,8 @@
       <c r="BE20"/>
       <c r="BF20"/>
     </row>
-    <row r="21" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="AD21" s="47" t="s">
+    <row r="21" spans="2:65">
+      <c r="AD21" s="43" t="s">
         <v>31</v>
       </c>
       <c r="AE21" s="32" t="s">
@@ -20880,7 +20941,7 @@
       <c r="BE21"/>
       <c r="BF21"/>
     </row>
-    <row r="22" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:65">
       <c r="AD22"/>
       <c r="AE22"/>
       <c r="AF22"/>
@@ -20900,7 +20961,7 @@
       <c r="BE22"/>
       <c r="BF22"/>
     </row>
-    <row r="23" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:65">
       <c r="AI23"/>
       <c r="AJ23"/>
       <c r="AK23"/>
@@ -20920,7 +20981,7 @@
       <c r="BE23"/>
       <c r="BF23"/>
     </row>
-    <row r="24" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:65">
       <c r="AI24"/>
       <c r="AJ24"/>
       <c r="AK24"/>
@@ -20939,7 +21000,7 @@
       <c r="BD24"/>
       <c r="BE24"/>
     </row>
-    <row r="25" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:65">
       <c r="V25" s="7"/>
       <c r="AJ25"/>
       <c r="AK25"/>
@@ -20954,22 +21015,22 @@
       <c r="BI25" s="6"/>
       <c r="BJ25" s="38"/>
     </row>
-    <row r="26" spans="2:65" x14ac:dyDescent="0.3">
-      <c r="L26" s="45" t="s">
+    <row r="26" spans="2:65">
+      <c r="L26" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="M26" s="45"/>
-      <c r="N26" s="45"/>
-      <c r="P26" s="45" t="s">
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
+      <c r="P26" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="45"/>
-      <c r="T26" s="45" t="s">
+      <c r="Q26" s="46"/>
+      <c r="R26" s="46"/>
+      <c r="T26" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="U26" s="45"/>
-      <c r="V26" s="45"/>
+      <c r="U26" s="46"/>
+      <c r="V26" s="46"/>
       <c r="AJ26"/>
       <c r="AK26"/>
       <c r="AL26"/>
@@ -20980,7 +21041,7 @@
       <c r="AT26"/>
       <c r="AY26"/>
     </row>
-    <row r="27" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:65">
       <c r="L27" s="7" t="s">
         <v>24</v>
       </c>
@@ -20999,32 +21060,32 @@
       <c r="AM27"/>
       <c r="AN27"/>
       <c r="AO27"/>
-      <c r="AS27" s="45" t="s">
+      <c r="AS27" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="AT27" s="45"/>
-      <c r="AU27" s="45"/>
-      <c r="AV27" s="45"/>
-      <c r="AW27" s="45"/>
-      <c r="AX27" s="45"/>
-      <c r="AZ27" s="45" t="s">
+      <c r="AT27" s="46"/>
+      <c r="AU27" s="46"/>
+      <c r="AV27" s="46"/>
+      <c r="AW27" s="46"/>
+      <c r="AX27" s="46"/>
+      <c r="AZ27" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="BA27" s="45"/>
-      <c r="BB27" s="45"/>
-      <c r="BC27" s="45"/>
-      <c r="BD27" s="45"/>
-      <c r="BE27" s="45"/>
-      <c r="BG27" s="45" t="s">
+      <c r="BA27" s="46"/>
+      <c r="BB27" s="46"/>
+      <c r="BC27" s="46"/>
+      <c r="BD27" s="46"/>
+      <c r="BE27" s="46"/>
+      <c r="BG27" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="BH27" s="45"/>
-      <c r="BI27" s="45"/>
-      <c r="BJ27" s="45"/>
-      <c r="BK27" s="45"/>
-      <c r="BL27" s="45"/>
+      <c r="BH27" s="46"/>
+      <c r="BI27" s="46"/>
+      <c r="BJ27" s="46"/>
+      <c r="BK27" s="46"/>
+      <c r="BL27" s="46"/>
     </row>
-    <row r="28" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:65">
       <c r="L28"/>
       <c r="N28"/>
       <c r="P28"/>
@@ -21052,7 +21113,7 @@
       <c r="BH28"/>
       <c r="BI28"/>
     </row>
-    <row r="29" spans="2:65" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:65" customFormat="1" ht="13">
       <c r="B29" s="41" t="s">
         <v>1</v>
       </c>
@@ -21213,7 +21274,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:65">
       <c r="B30" t="s">
         <v>4</v>
       </c>
@@ -21333,9 +21394,9 @@
       <c r="AP30" t="s">
         <v>19</v>
       </c>
-      <c r="AQ30" s="9">
+      <c r="AQ30" s="9" t="e">
         <f ca="1">MAX(JS3_TabInd1[C])</f>
-        <v>19</v>
+        <v>#REF!</v>
       </c>
       <c r="AR30" s="9"/>
       <c r="AS30">
@@ -21414,7 +21475,7 @@
       </c>
       <c r="BM30"/>
     </row>
-    <row r="31" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:65">
       <c r="B31" t="s">
         <v>5</v>
       </c>
@@ -21515,28 +21576,28 @@
         <f>JS3_TabJob[[#This Row],[Job]]</f>
         <v>B</v>
       </c>
-      <c r="AK31" s="8">
+      <c r="AK31" s="8" t="e">
         <f t="array" aca="1" ref="AK31" ca="1">MAX(IF(JS3_TabOp[Job]=JS3_TabInd1[[#This Row],[Job]],JS3_TabOp[tf]))</f>
-        <v>14</v>
-      </c>
-      <c r="AL31" s="8">
+        <v>#REF!</v>
+      </c>
+      <c r="AL31" s="8" t="e">
         <f ca="1">AK31-C31</f>
-        <v>14</v>
-      </c>
-      <c r="AM31">
+        <v>#REF!</v>
+      </c>
+      <c r="AM31" t="e">
         <f ca="1">AK31-D31</f>
-        <v>4</v>
-      </c>
-      <c r="AN31">
+        <v>#REF!</v>
+      </c>
+      <c r="AN31" t="e">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>#REF!</v>
       </c>
       <c r="AP31" t="s">
         <v>18</v>
       </c>
-      <c r="AQ31" s="9">
+      <c r="AQ31" s="9" t="e">
         <f ca="1">AVERAGE(JS3_TabInd1[F])</f>
-        <v>10</v>
+        <v>#REF!</v>
       </c>
       <c r="AR31" s="9"/>
       <c r="AS31">
@@ -21547,21 +21608,21 @@
         <f t="shared" si="2"/>
         <v>B</v>
       </c>
-      <c r="AU31">
+      <c r="AU31" t="e">
         <f ca="1">IF(AS31="","",VLOOKUP(JS3_TabM1[[#This Row],[Op]],JS3_TabOp[],10))</f>
-        <v>2</v>
-      </c>
-      <c r="AV31">
+        <v>#REF!</v>
+      </c>
+      <c r="AV31" t="e">
         <f ca="1">IF(AS31="","",VLOOKUP(AS31,JS3_TabOp[],11))</f>
-        <v>3</v>
-      </c>
-      <c r="AW31">
+        <v>#REF!</v>
+      </c>
+      <c r="AW31" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AX31">
+        <v>#REF!</v>
+      </c>
+      <c r="AX31" t="e">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>#REF!</v>
       </c>
       <c r="AY31"/>
       <c r="AZ31">
@@ -21572,21 +21633,21 @@
         <f t="shared" si="6"/>
         <v>B</v>
       </c>
-      <c r="BB31">
+      <c r="BB31" t="e">
         <f ca="1">IF(AZ31="","",VLOOKUP(JS3_TabM2[[#This Row],[Op]],JS3_TabOp[],10))</f>
-        <v>3</v>
-      </c>
-      <c r="BC31">
+        <v>#REF!</v>
+      </c>
+      <c r="BC31" t="e">
         <f ca="1">IF(AZ31="","",VLOOKUP(AZ31,JS3_TabOp[],11))</f>
-        <v>6</v>
-      </c>
-      <c r="BD31">
+        <v>#REF!</v>
+      </c>
+      <c r="BD31" t="e">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="BE31">
+        <v>#REF!</v>
+      </c>
+      <c r="BE31" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>#REF!</v>
       </c>
       <c r="BF31"/>
       <c r="BG31">
@@ -21597,25 +21658,25 @@
         <f t="shared" si="10"/>
         <v>C</v>
       </c>
-      <c r="BI31">
+      <c r="BI31" t="e">
         <f ca="1">IF(BG31="","",VLOOKUP(JS3_TabM3[[#This Row],[Op]],JS3_TabOp[],10))</f>
-        <v>7</v>
-      </c>
-      <c r="BJ31">
+        <v>#REF!</v>
+      </c>
+      <c r="BJ31" t="e">
         <f ca="1">IF(BG31="","",VLOOKUP(BG31,JS3_TabOp[],11))</f>
-        <v>10</v>
-      </c>
-      <c r="BK31">
+        <v>#REF!</v>
+      </c>
+      <c r="BK31" t="e">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="BL31">
+        <v>#REF!</v>
+      </c>
+      <c r="BL31" t="e">
         <f t="shared" ca="1" si="12"/>
-        <v>3</v>
+        <v>#REF!</v>
       </c>
       <c r="BM31"/>
     </row>
-    <row r="32" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:65">
       <c r="B32" t="s">
         <v>3</v>
       </c>
@@ -21691,9 +21752,9 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD32">
+      <c r="AD32" t="e">
         <f t="shared" ca="1" si="14"/>
-        <v>1</v>
+        <v>#REF!</v>
       </c>
       <c r="AE32">
         <f>IF(AC32=0,VLOOKUP(Y32,JS3_TabJob[],2),"")</f>
@@ -21703,41 +21764,41 @@
         <f>VLOOKUP(Y32,JS3_TabJob[],3,0)</f>
         <v>10</v>
       </c>
-      <c r="AG32">
+      <c r="AG32" t="e">
         <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AH32">
+        <v>#REF!</v>
+      </c>
+      <c r="AH32" t="e">
         <f ca="1">JS3_TabOp[[#This Row],[ti]]+JS3_TabOp[[#This Row],[p]]</f>
-        <v>3</v>
+        <v>#REF!</v>
       </c>
       <c r="AI32"/>
       <c r="AJ32" t="str">
         <f>JS3_TabJob[[#This Row],[Job]]</f>
         <v>C</v>
       </c>
-      <c r="AK32" s="8">
+      <c r="AK32" s="8" t="e">
         <f t="array" aca="1" ref="AK32" ca="1">MAX(IF(JS3_TabOp[Job]=JS3_TabInd1[[#This Row],[Job]],JS3_TabOp[tf]))</f>
-        <v>10</v>
-      </c>
-      <c r="AL32" s="8">
+        <v>#REF!</v>
+      </c>
+      <c r="AL32" s="8" t="e">
         <f ca="1">AK32-C32</f>
-        <v>10</v>
-      </c>
-      <c r="AM32">
+        <v>#REF!</v>
+      </c>
+      <c r="AM32" t="e">
         <f ca="1">AK32-D32</f>
-        <v>0</v>
-      </c>
-      <c r="AN32">
+        <v>#REF!</v>
+      </c>
+      <c r="AN32" t="e">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="AP32" t="s">
         <v>20</v>
       </c>
-      <c r="AQ32" s="9">
+      <c r="AQ32" s="9" t="e">
         <f ca="1">SUM(JS3_TabInd1[T])</f>
-        <v>8</v>
+        <v>#REF!</v>
       </c>
       <c r="AR32" s="9"/>
       <c r="AS32">
@@ -21748,21 +21809,21 @@
         <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="AU32">
+      <c r="AU32" t="e">
         <f ca="1">IF(AS32="","",VLOOKUP(JS3_TabM1[[#This Row],[Op]],JS3_TabOp[],10))</f>
-        <v>5</v>
-      </c>
-      <c r="AV32">
+        <v>#REF!</v>
+      </c>
+      <c r="AV32" t="e">
         <f ca="1">IF(AS32="","",VLOOKUP(AS32,JS3_TabOp[],11))</f>
-        <v>7</v>
-      </c>
-      <c r="AW32">
+        <v>#REF!</v>
+      </c>
+      <c r="AW32" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="AX32">
+        <v>#REF!</v>
+      </c>
+      <c r="AX32" t="e">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>#REF!</v>
       </c>
       <c r="AY32"/>
       <c r="AZ32">
@@ -21773,21 +21834,21 @@
         <f t="shared" si="6"/>
         <v>D</v>
       </c>
-      <c r="BB32">
+      <c r="BB32" t="e">
         <f ca="1">IF(AZ32="","",VLOOKUP(JS3_TabM2[[#This Row],[Op]],JS3_TabOp[],10))</f>
-        <v>7</v>
-      </c>
-      <c r="BC32">
+        <v>#REF!</v>
+      </c>
+      <c r="BC32" t="e">
         <f ca="1">IF(AZ32="","",VLOOKUP(AZ32,JS3_TabOp[],11))</f>
-        <v>10</v>
-      </c>
-      <c r="BD32">
+        <v>#REF!</v>
+      </c>
+      <c r="BD32" t="e">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="BE32">
+        <v>#REF!</v>
+      </c>
+      <c r="BE32" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>#REF!</v>
       </c>
       <c r="BF32"/>
       <c r="BG32">
@@ -21798,25 +21859,25 @@
         <f t="shared" si="10"/>
         <v>B</v>
       </c>
-      <c r="BI32">
+      <c r="BI32" t="e">
         <f ca="1">IF(BG32="","",VLOOKUP(JS3_TabM3[[#This Row],[Op]],JS3_TabOp[],10))</f>
-        <v>10</v>
-      </c>
-      <c r="BJ32">
+        <v>#REF!</v>
+      </c>
+      <c r="BJ32" t="e">
         <f ca="1">IF(BG32="","",VLOOKUP(BG32,JS3_TabOp[],11))</f>
-        <v>14</v>
-      </c>
-      <c r="BK32">
+        <v>#REF!</v>
+      </c>
+      <c r="BK32" t="e">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="BL32">
+        <v>#REF!</v>
+      </c>
+      <c r="BL32" t="e">
         <f t="shared" ca="1" si="12"/>
-        <v>4</v>
+        <v>#REF!</v>
       </c>
       <c r="BM32"/>
     </row>
-    <row r="33" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:65">
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -21886,9 +21947,9 @@
         <f t="shared" si="13"/>
         <v>3</v>
       </c>
-      <c r="AD33">
+      <c r="AD33" t="e">
         <f t="shared" ca="1" si="14"/>
-        <v>6</v>
+        <v>#REF!</v>
       </c>
       <c r="AE33" t="str">
         <f>IF(AC33=0,VLOOKUP(Y33,JS3_TabJob[],2),"")</f>
@@ -21898,41 +21959,41 @@
         <f>VLOOKUP(Y33,JS3_TabJob[],3,0)</f>
         <v>10</v>
       </c>
-      <c r="AG33">
+      <c r="AG33" t="e">
         <f t="shared" ca="1" si="15"/>
-        <v>3</v>
-      </c>
-      <c r="AH33">
+        <v>#REF!</v>
+      </c>
+      <c r="AH33" t="e">
         <f ca="1">JS3_TabOp[[#This Row],[ti]]+JS3_TabOp[[#This Row],[p]]</f>
-        <v>6</v>
+        <v>#REF!</v>
       </c>
       <c r="AI33"/>
       <c r="AJ33" t="str">
         <f>JS3_TabJob[[#This Row],[Job]]</f>
         <v>D</v>
       </c>
-      <c r="AK33" s="8">
+      <c r="AK33" s="8" t="e">
         <f t="array" aca="1" ref="AK33" ca="1">MAX(IF(JS3_TabOp[Job]=JS3_TabInd1[[#This Row],[Job]],JS3_TabOp[tf]))</f>
-        <v>10</v>
-      </c>
-      <c r="AL33" s="8">
+        <v>#REF!</v>
+      </c>
+      <c r="AL33" s="8" t="e">
         <f ca="1">AK33-C33</f>
-        <v>5</v>
-      </c>
-      <c r="AM33">
+        <v>#REF!</v>
+      </c>
+      <c r="AM33" t="e">
         <f ca="1">AK33-D33</f>
-        <v>-5</v>
-      </c>
-      <c r="AN33">
+        <v>#REF!</v>
+      </c>
+      <c r="AN33" t="e">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="AP33" t="s">
         <v>21</v>
       </c>
-      <c r="AQ33" s="9">
+      <c r="AQ33" s="9" t="e">
         <f ca="1">MAX(JS3_TabInd1[T])</f>
-        <v>4</v>
+        <v>#REF!</v>
       </c>
       <c r="AR33" s="9"/>
       <c r="AS33">
@@ -21943,21 +22004,21 @@
         <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="AU33">
+      <c r="AU33" t="e">
         <f ca="1">IF(AS33="","",VLOOKUP(JS3_TabM1[[#This Row],[Op]],JS3_TabOp[],10))</f>
-        <v>7</v>
-      </c>
-      <c r="AV33">
+        <v>#REF!</v>
+      </c>
+      <c r="AV33" t="e">
         <f ca="1">IF(AS33="","",VLOOKUP(AS33,JS3_TabOp[],11))</f>
-        <v>9</v>
-      </c>
-      <c r="AW33">
+        <v>#REF!</v>
+      </c>
+      <c r="AW33" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AX33">
+        <v>#REF!</v>
+      </c>
+      <c r="AX33" t="e">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>#REF!</v>
       </c>
       <c r="AY33"/>
       <c r="AZ33" t="str">
@@ -21993,25 +22054,25 @@
         <f t="shared" si="10"/>
         <v>E</v>
       </c>
-      <c r="BI33">
+      <c r="BI33" t="e">
         <f ca="1">IF(BG33="","",VLOOKUP(JS3_TabM3[[#This Row],[Op]],JS3_TabOp[],10))</f>
-        <v>14</v>
-      </c>
-      <c r="BJ33">
+        <v>#REF!</v>
+      </c>
+      <c r="BJ33" t="e">
         <f ca="1">IF(BG33="","",VLOOKUP(BG33,JS3_TabOp[],11))</f>
-        <v>19</v>
-      </c>
-      <c r="BK33">
+        <v>#REF!</v>
+      </c>
+      <c r="BK33" t="e">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="BL33">
+        <v>#REF!</v>
+      </c>
+      <c r="BL33" t="e">
         <f t="shared" ca="1" si="12"/>
-        <v>5</v>
+        <v>#REF!</v>
       </c>
       <c r="BM33"/>
     </row>
-    <row r="34" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:65">
       <c r="B34" t="s">
         <v>7</v>
       </c>
@@ -22069,9 +22130,9 @@
         <f t="shared" si="13"/>
         <v>4</v>
       </c>
-      <c r="AD34">
+      <c r="AD34" t="e">
         <f t="shared" ca="1" si="14"/>
-        <v>7</v>
+        <v>#REF!</v>
       </c>
       <c r="AE34" t="str">
         <f>IF(AC34=0,VLOOKUP(Y34,JS3_TabJob[],2),"")</f>
@@ -22081,41 +22142,41 @@
         <f>VLOOKUP(Y34,JS3_TabJob[],3,0)</f>
         <v>10</v>
       </c>
-      <c r="AG34">
+      <c r="AG34" t="e">
         <f t="shared" ca="1" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="AH34">
+        <v>#REF!</v>
+      </c>
+      <c r="AH34" t="e">
         <f ca="1">JS3_TabOp[[#This Row],[ti]]+JS3_TabOp[[#This Row],[p]]</f>
-        <v>14</v>
+        <v>#REF!</v>
       </c>
       <c r="AI34"/>
       <c r="AJ34" t="str">
         <f>JS3_TabJob[[#This Row],[Job]]</f>
         <v>E</v>
       </c>
-      <c r="AK34" s="8">
+      <c r="AK34" s="8" t="e">
         <f t="array" aca="1" ref="AK34" ca="1">MAX(IF(JS3_TabOp[Job]=JS3_TabInd1[[#This Row],[Job]],JS3_TabOp[tf]))</f>
-        <v>19</v>
-      </c>
-      <c r="AL34" s="8">
+        <v>#REF!</v>
+      </c>
+      <c r="AL34" s="8" t="e">
         <f ca="1">AK34-C34</f>
-        <v>14</v>
-      </c>
-      <c r="AM34">
+        <v>#REF!</v>
+      </c>
+      <c r="AM34" t="e">
         <f ca="1">AK34-D34</f>
-        <v>4</v>
-      </c>
-      <c r="AN34">
+        <v>#REF!</v>
+      </c>
+      <c r="AN34" t="e">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>#REF!</v>
       </c>
       <c r="AP34" t="s">
         <v>22</v>
       </c>
       <c r="AQ34" s="25">
         <f ca="1">COUNTIF(JS3_TabInd1[T],"&gt;0")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR34" s="9"/>
       <c r="AS34" t="str">
@@ -22194,7 +22255,7 @@
       </c>
       <c r="BM34"/>
     </row>
-    <row r="35" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:65">
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
@@ -22347,7 +22408,7 @@
       </c>
       <c r="BM35"/>
     </row>
-    <row r="36" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:65">
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
@@ -22396,9 +22457,9 @@
         <f t="shared" si="13"/>
         <v>6</v>
       </c>
-      <c r="AD36">
+      <c r="AD36" t="e">
         <f t="shared" ca="1" si="14"/>
-        <v>2</v>
+        <v>#REF!</v>
       </c>
       <c r="AE36" t="str">
         <f>IF(AC36=0,VLOOKUP(Y36,JS3_TabJob[],2),"")</f>
@@ -22408,13 +22469,13 @@
         <f>VLOOKUP(Y36,JS3_TabJob[],3,0)</f>
         <v>10</v>
       </c>
-      <c r="AG36">
+      <c r="AG36" t="e">
         <f t="shared" ca="1" si="15"/>
-        <v>7</v>
-      </c>
-      <c r="AH36">
+        <v>#REF!</v>
+      </c>
+      <c r="AH36" t="e">
         <f ca="1">JS3_TabOp[[#This Row],[ti]]+JS3_TabOp[[#This Row],[p]]</f>
-        <v>10</v>
+        <v>#REF!</v>
       </c>
       <c r="AI36"/>
       <c r="AK36"/>
@@ -22501,7 +22562,7 @@
       </c>
       <c r="BM36"/>
     </row>
-    <row r="37" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:65">
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
@@ -22550,9 +22611,9 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD37">
+      <c r="AD37" t="e">
         <f t="shared" ca="1" si="14"/>
-        <v>3</v>
+        <v>#REF!</v>
       </c>
       <c r="AE37">
         <f>IF(AC37=0,VLOOKUP(Y37,JS3_TabJob[],2),"")</f>
@@ -22562,13 +22623,13 @@
         <f>VLOOKUP(Y37,JS3_TabJob[],3,0)</f>
         <v>15</v>
       </c>
-      <c r="AG37">
+      <c r="AG37" t="e">
         <f t="shared" ca="1" si="15"/>
-        <v>5</v>
-      </c>
-      <c r="AH37">
+        <v>#REF!</v>
+      </c>
+      <c r="AH37" t="e">
         <f ca="1">JS3_TabOp[[#This Row],[ti]]+JS3_TabOp[[#This Row],[p]]</f>
-        <v>7</v>
+        <v>#REF!</v>
       </c>
       <c r="AI37"/>
       <c r="AK37"/>
@@ -22655,7 +22716,7 @@
       </c>
       <c r="BM37"/>
     </row>
-    <row r="38" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:65">
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
@@ -22704,9 +22765,9 @@
         <f t="shared" si="13"/>
         <v>8</v>
       </c>
-      <c r="AD38">
+      <c r="AD38" t="e">
         <f t="shared" ca="1" si="14"/>
-        <v>4</v>
+        <v>#REF!</v>
       </c>
       <c r="AE38" t="str">
         <f>IF(AC38=0,VLOOKUP(Y38,JS3_TabJob[],2),"")</f>
@@ -22716,13 +22777,13 @@
         <f>VLOOKUP(Y38,JS3_TabJob[],3,0)</f>
         <v>15</v>
       </c>
-      <c r="AG38">
+      <c r="AG38" t="e">
         <f t="shared" ca="1" si="15"/>
-        <v>7</v>
-      </c>
-      <c r="AH38">
+        <v>#REF!</v>
+      </c>
+      <c r="AH38" t="e">
         <f ca="1">JS3_TabOp[[#This Row],[ti]]+JS3_TabOp[[#This Row],[p]]</f>
-        <v>10</v>
+        <v>#REF!</v>
       </c>
       <c r="AI38"/>
       <c r="AK38"/>
@@ -22809,7 +22870,7 @@
       </c>
       <c r="BM38"/>
     </row>
-    <row r="39" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:65">
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
@@ -22858,9 +22919,9 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD39">
+      <c r="AD39" t="e">
         <f t="shared" ca="1" si="14"/>
-        <v>8</v>
+        <v>#REF!</v>
       </c>
       <c r="AE39">
         <f>IF(AC39=0,VLOOKUP(Y39,JS3_TabJob[],2),"")</f>
@@ -22870,13 +22931,13 @@
         <f>VLOOKUP(Y39,JS3_TabJob[],3,0)</f>
         <v>15</v>
       </c>
-      <c r="AG39">
+      <c r="AG39" t="e">
         <f t="shared" ca="1" si="15"/>
-        <v>7</v>
-      </c>
-      <c r="AH39">
+        <v>#REF!</v>
+      </c>
+      <c r="AH39" t="e">
         <f ca="1">JS3_TabOp[[#This Row],[ti]]+JS3_TabOp[[#This Row],[p]]</f>
-        <v>9</v>
+        <v>#REF!</v>
       </c>
       <c r="AI39"/>
       <c r="AK39"/>
@@ -22963,7 +23024,7 @@
       </c>
       <c r="BM39"/>
     </row>
-    <row r="40" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:65">
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
@@ -23006,9 +23067,9 @@
         <f t="shared" si="13"/>
         <v>10</v>
       </c>
-      <c r="AD40">
+      <c r="AD40" t="e">
         <f t="shared" ca="1" si="14"/>
-        <v>5</v>
+        <v>#REF!</v>
       </c>
       <c r="AE40" t="str">
         <f>IF(AC40=0,VLOOKUP(Y40,JS3_TabJob[],2),"")</f>
@@ -23018,13 +23079,13 @@
         <f>VLOOKUP(Y40,JS3_TabJob[],3,0)</f>
         <v>15</v>
       </c>
-      <c r="AG40">
+      <c r="AG40" t="e">
         <f t="shared" ca="1" si="15"/>
-        <v>14</v>
-      </c>
-      <c r="AH40">
+        <v>#REF!</v>
+      </c>
+      <c r="AH40" t="e">
         <f ca="1">JS3_TabOp[[#This Row],[ti]]+JS3_TabOp[[#This Row],[p]]</f>
-        <v>19</v>
+        <v>#REF!</v>
       </c>
       <c r="AI40"/>
       <c r="AK40"/>
@@ -23040,7 +23101,7 @@
       <c r="BF40"/>
       <c r="BJ40"/>
     </row>
-    <row r="41" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:65">
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
@@ -23071,7 +23132,7 @@
       <c r="BC41"/>
       <c r="BD41"/>
     </row>
-    <row r="42" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:65">
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42"/>
@@ -23104,7 +23165,7 @@
       <c r="BB42"/>
       <c r="BD42"/>
     </row>
-    <row r="43" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:65">
       <c r="B43"/>
       <c r="C43"/>
       <c r="D43"/>
@@ -23145,7 +23206,7 @@
       <c r="BF43"/>
       <c r="BG43"/>
     </row>
-    <row r="44" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:65">
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
@@ -23186,7 +23247,7 @@
       <c r="BF44"/>
       <c r="BG44"/>
     </row>
-    <row r="45" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:65">
       <c r="B45"/>
       <c r="C45"/>
       <c r="D45"/>
@@ -23227,7 +23288,7 @@
       <c r="BF45"/>
       <c r="BG45"/>
     </row>
-    <row r="46" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:65">
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
@@ -23254,7 +23315,7 @@
       <c r="BF46"/>
       <c r="BG46"/>
     </row>
-    <row r="47" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:65">
       <c r="B47"/>
       <c r="C47"/>
       <c r="D47"/>
@@ -23270,7 +23331,7 @@
       <c r="AF47"/>
       <c r="AI47"/>
     </row>
-    <row r="48" spans="2:65" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:65">
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
@@ -23286,7 +23347,7 @@
       <c r="AF48"/>
       <c r="AI48"/>
     </row>
-    <row r="49" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:37">
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
@@ -23302,7 +23363,7 @@
       <c r="AF49"/>
       <c r="AI49"/>
     </row>
-    <row r="50" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:37">
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50"/>
@@ -23318,7 +23379,7 @@
       <c r="AF50"/>
       <c r="AI50"/>
     </row>
-    <row r="51" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:37">
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
@@ -23336,7 +23397,7 @@
       <c r="AJ51"/>
       <c r="AK51"/>
     </row>
-    <row r="52" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:37">
       <c r="W52"/>
       <c r="X52"/>
       <c r="Y52"/>
@@ -23351,7 +23412,7 @@
       <c r="AJ52"/>
       <c r="AK52"/>
     </row>
-    <row r="53" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:37">
       <c r="W53"/>
       <c r="X53"/>
       <c r="Y53"/>
@@ -23403,15 +23464,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="26" width="5.6640625" style="13" customWidth="1"/>
-    <col min="27" max="27" width="20.6640625" style="13" customWidth="1"/>
-    <col min="28" max="46" width="5.6640625" style="13" customWidth="1"/>
-    <col min="47" max="16384" width="8.88671875" style="13"/>
+    <col min="1" max="26" width="5.6328125" style="13" customWidth="1"/>
+    <col min="27" max="27" width="20.6328125" style="13" customWidth="1"/>
+    <col min="28" max="46" width="5.6328125" style="13" customWidth="1"/>
+    <col min="47" max="16384" width="8.90625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="12" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:39" s="12" customFormat="1" ht="26">
       <c r="A1" s="10" t="s">
         <v>39</v>
       </c>
@@ -23439,7 +23500,7 @@
       <c r="W1" s="10"/>
       <c r="X1" s="10"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39">
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -23458,7 +23519,7 @@
       <c r="AG3"/>
       <c r="AH3"/>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39">
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -23475,7 +23536,7 @@
       <c r="AL4" s="15"/>
       <c r="AM4" s="15"/>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -23491,7 +23552,7 @@
       <c r="AI5" s="15"/>
       <c r="AJ5" s="15"/>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39">
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -23507,7 +23568,7 @@
       <c r="AI6" s="15"/>
       <c r="AJ6" s="15"/>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -23521,7 +23582,7 @@
       <c r="AG7"/>
       <c r="AH7"/>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39">
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -23535,7 +23596,7 @@
       <c r="AG8"/>
       <c r="AH8"/>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -23549,7 +23610,7 @@
       <c r="AG9"/>
       <c r="AH9"/>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39">
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -23567,7 +23628,7 @@
       <c r="AG10"/>
       <c r="AH10"/>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -23586,7 +23647,7 @@
       <c r="AG11"/>
       <c r="AH11"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39">
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -23605,7 +23666,7 @@
       <c r="AG12"/>
       <c r="AH12"/>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -23624,25 +23685,25 @@
       <c r="AG13" s="15"/>
       <c r="AH13" s="15"/>
     </row>
-    <row r="26" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:40">
       <c r="B26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="46" t="s">
+      <c r="I26" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46"/>
-      <c r="M26" s="46" t="s">
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="M26" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="N26" s="46"/>
-      <c r="O26" s="46"/>
-      <c r="Q26" s="46" t="s">
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="Q26" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="R26" s="46"/>
-      <c r="S26" s="46"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="47"/>
       <c r="U26" s="21"/>
       <c r="V26" s="21"/>
       <c r="W26" s="21"/>
@@ -23652,24 +23713,24 @@
       <c r="AA26" s="21"/>
       <c r="AB26" s="21"/>
       <c r="AC26" s="21"/>
-      <c r="AD26" s="43" t="s">
+      <c r="AD26" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="AE26" s="43"/>
-      <c r="AF26" s="43"/>
+      <c r="AE26" s="44"/>
+      <c r="AF26" s="44"/>
       <c r="AG26" s="15"/>
-      <c r="AH26" s="43" t="s">
+      <c r="AH26" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="AI26" s="43"/>
-      <c r="AJ26" s="43"/>
-      <c r="AL26" s="43" t="s">
+      <c r="AI26" s="44"/>
+      <c r="AJ26" s="44"/>
+      <c r="AL26" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="AM26" s="43"/>
-      <c r="AN26" s="43"/>
+      <c r="AM26" s="44"/>
+      <c r="AN26" s="44"/>
     </row>
-    <row r="27" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:40">
       <c r="B27" s="15"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
@@ -23692,7 +23753,7 @@
       <c r="AG27" s="15"/>
       <c r="AH27" s="15"/>
     </row>
-    <row r="28" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:40">
       <c r="B28" s="39" t="s">
         <v>0</v>
       </c>
@@ -23791,7 +23852,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:40">
       <c r="B29" s="15"/>
       <c r="C29" s="15" t="s">
         <v>4</v>
@@ -23912,7 +23973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:40">
       <c r="B30" s="15"/>
       <c r="C30" s="15" t="s">
         <v>5</v>
@@ -24033,7 +24094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:40">
       <c r="B31" s="15"/>
       <c r="C31" s="15" t="s">
         <v>3</v>
@@ -24154,7 +24215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:40">
       <c r="B32" s="15"/>
       <c r="C32" s="15" t="s">
         <v>6</v>
@@ -24275,7 +24336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:40">
       <c r="B33" s="15"/>
       <c r="C33" s="15" t="s">
         <v>7</v>
@@ -24396,7 +24457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:40">
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
@@ -24431,7 +24492,7 @@
       <c r="AG34" s="15"/>
       <c r="AH34" s="15"/>
     </row>
-    <row r="35" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:40">
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
@@ -24463,7 +24524,7 @@
       <c r="AG35" s="26"/>
       <c r="AH35" s="26"/>
     </row>
-    <row r="36" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:40">
       <c r="B36" s="24"/>
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
@@ -24490,7 +24551,7 @@
       <c r="AB36" s="14"/>
       <c r="AC36" s="14"/>
     </row>
-    <row r="37" spans="2:40" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:40">
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
       <c r="D37" s="14"/>

</xml_diff>

<commit_message>
Tarefa 2 - Aula 2 NAO FINALIIZADA
</commit_message>
<xml_diff>
--- a/Aula 1/3515 L01 Sched 2020.xlsx
+++ b/Aula 1/3515 L01 Sched 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thale\Documents\Faculdade\PRO3515 - Algoritmos de Otimização para Problemas de Programação da Produção\Aula 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C662B2-E8C5-4FCC-9928-4884AF444022}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4B6F24-5D21-4AC0-9B38-90AFCCA96A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1095" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M1" sheetId="30" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="52">
   <si>
     <t>#</t>
   </si>
@@ -444,6 +444,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,12 +460,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1661,7 +1661,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>D</c:v>
+                  <c:v>E</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1718,7 +1718,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1777,7 +1777,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>E</c:v>
+                  <c:v>A</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1834,7 +1834,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1893,7 +1893,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A</c:v>
+                  <c:v>C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1950,7 +1950,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2009,7 +2009,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C</c:v>
+                  <c:v>D</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2066,7 +2066,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2182,7 +2182,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15253,10 +15253,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="M1_Tab0" displayName="M1_Tab0" ref="B14:E20" totalsRowShown="0" headerRowDxfId="115">
-  <autoFilter ref="B14:E20" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B15:E20">
-    <sortCondition ref="B14:B20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="M1_Tab0" displayName="M1_Tab0" ref="B14:E19" totalsRowShown="0" headerRowDxfId="115">
+  <autoFilter ref="B14:E19" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B15:E19">
+    <sortCondition ref="B14:B19"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#"/>
@@ -15442,8 +15442,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="M1_Tab1" displayName="M1_Tab1" ref="G14:I20" totalsRowShown="0" headerRowDxfId="114">
-  <autoFilter ref="G14:I20" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="M1_Tab1" displayName="M1_Tab1" ref="G14:I19" totalsRowShown="0" headerRowDxfId="114">
+  <autoFilter ref="G14:I19" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Job">
       <calculatedColumnFormula>C15</calculatedColumnFormula>
@@ -15642,8 +15642,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="M1_Tab2" displayName="M1_Tab2" ref="K14:O20" totalsRowShown="0" headerRowDxfId="113">
-  <autoFilter ref="K14:O20" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="M1_Tab2" displayName="M1_Tab2" ref="K14:O19" totalsRowShown="0" headerRowDxfId="113">
+  <autoFilter ref="K14:O19" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K17:O21">
     <sortCondition ref="K15:K20"/>
   </sortState>
@@ -15867,8 +15867,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="M1_Tab4" displayName="M1_Tab4" ref="T14:V20" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
-  <autoFilter ref="T14:V20" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="M1_Tab4" displayName="M1_Tab4" ref="T14:V19" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
+  <autoFilter ref="T14:V19" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Job" dataDxfId="110">
       <calculatedColumnFormula>G15</calculatedColumnFormula>
@@ -16370,8 +16370,8 @@
   </sheetPr>
   <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -16533,11 +16533,11 @@
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
       <c r="S12" s="15"/>
-      <c r="T12" s="44" t="s">
+      <c r="T12" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="U12" s="44"/>
-      <c r="V12" s="44"/>
+      <c r="U12" s="46"/>
+      <c r="V12" s="46"/>
       <c r="W12" s="15"/>
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
@@ -16625,50 +16625,48 @@
       </c>
     </row>
     <row r="15" spans="1:32">
-      <c r="B15" s="15">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="15">
         <v>1</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="15">
+      <c r="E15" s="15">
         <v>4</v>
-      </c>
-      <c r="E15" s="15">
-        <v>18</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15" t="str">
-        <f>C15</f>
-        <v>D</v>
+        <f t="shared" ref="G15:G20" si="0">C15</f>
+        <v>E</v>
       </c>
       <c r="H15" s="15">
-        <f>IF(ISNUMBER(I14),I14,0)</f>
+        <f t="shared" ref="H15:H20" si="1">IF(ISNUMBER(I14),I14,0)</f>
         <v>0</v>
       </c>
       <c r="I15" s="15">
-        <f>H15+D15</f>
-        <v>4</v>
+        <f t="shared" ref="I15:I20" si="2">H15+D15</f>
+        <v>1</v>
       </c>
       <c r="J15" s="15"/>
       <c r="K15" s="15" t="str">
-        <f>G15</f>
-        <v>D</v>
+        <f t="shared" ref="K15:K20" si="3">G15</f>
+        <v>E</v>
       </c>
       <c r="L15" s="15">
-        <f>I15</f>
+        <f t="shared" ref="L15:L20" si="4">I15</f>
+        <v>1</v>
+      </c>
+      <c r="M15" s="15">
+        <f t="shared" ref="M15:M20" si="5">E15</f>
         <v>4</v>
       </c>
-      <c r="M15" s="15">
-        <f>E15</f>
-        <v>18</v>
-      </c>
       <c r="N15" s="15">
-        <f>L15-M15</f>
-        <v>-14</v>
+        <f t="shared" ref="N15:N20" si="6">L15-M15</f>
+        <v>-3</v>
       </c>
       <c r="O15" s="15">
-        <f>MAX(0,N15)</f>
+        <f t="shared" ref="O15:O20" si="7">MAX(0,N15)</f>
         <v>0</v>
       </c>
       <c r="Q15" t="s">
@@ -16676,11 +16674,11 @@
       </c>
       <c r="R15" s="9">
         <f>MAX(M1_Tab2[C])</f>
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="T15" s="17" t="str">
         <f>G15</f>
-        <v>D</v>
+        <v>E</v>
       </c>
       <c r="U15" s="35">
         <f>H15</f>
@@ -16688,56 +16686,54 @@
       </c>
       <c r="V15" s="35">
         <f>I15-H15</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W15" s="15"/>
       <c r="X15" s="15"/>
     </row>
     <row r="16" spans="1:32">
-      <c r="B16" s="15">
-        <v>2</v>
-      </c>
+      <c r="B16" s="15"/>
       <c r="C16" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="15">
+        <v>3</v>
+      </c>
+      <c r="E16" s="15">
         <v>7</v>
-      </c>
-      <c r="D16" s="15">
-        <v>5</v>
-      </c>
-      <c r="E16" s="15">
-        <v>17</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15" t="str">
-        <f>C16</f>
-        <v>E</v>
+        <f t="shared" si="0"/>
+        <v>A</v>
       </c>
       <c r="H16" s="15">
-        <f>IF(ISNUMBER(I15),I15,0)</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="15">
+        <f t="shared" si="2"/>
         <v>4</v>
-      </c>
-      <c r="I16" s="15">
-        <f>H16+D16</f>
-        <v>9</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15" t="str">
-        <f>G16</f>
-        <v>E</v>
+        <f t="shared" si="3"/>
+        <v>A</v>
       </c>
       <c r="L16" s="15">
-        <f>I16</f>
-        <v>9</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="M16" s="15">
-        <f>E16</f>
-        <v>17</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="N16" s="15">
-        <f>L16-M16</f>
-        <v>-8</v>
+        <f t="shared" si="6"/>
+        <v>-3</v>
       </c>
       <c r="O16" s="15">
-        <f>MAX(0,N16)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q16" t="s">
@@ -16745,68 +16741,66 @@
       </c>
       <c r="R16" s="9">
         <f>AVERAGE(M1_Tab2[C])</f>
-        <v>14.5</v>
+        <v>7.8</v>
       </c>
       <c r="T16" s="17" t="str">
         <f>G16</f>
-        <v>E</v>
+        <v>A</v>
       </c>
       <c r="U16" s="35">
-        <f t="shared" ref="U16:U19" si="0">H16-I15</f>
+        <f t="shared" ref="U16:U19" si="8">H16-I15</f>
         <v>0</v>
       </c>
       <c r="V16" s="35">
-        <f t="shared" ref="V16:V19" si="1">I16-H16</f>
-        <v>5</v>
+        <f t="shared" ref="V16:V19" si="9">I16-H16</f>
+        <v>3</v>
       </c>
       <c r="W16" s="15"/>
       <c r="X16" s="15"/>
     </row>
     <row r="17" spans="2:32">
-      <c r="B17" s="15">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>4</v>
-      </c>
       <c r="D17" s="15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E17" s="15">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15" t="str">
-        <f>C17</f>
-        <v>A</v>
+        <f t="shared" si="0"/>
+        <v>C</v>
       </c>
       <c r="H17" s="15">
-        <f>IF(ISNUMBER(I16),I16,0)</f>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="I17" s="15">
-        <f>H17+D17</f>
-        <v>15</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15" t="str">
-        <f>G17</f>
-        <v>A</v>
+        <f t="shared" si="3"/>
+        <v>C</v>
       </c>
       <c r="L17" s="15">
-        <f>I17</f>
-        <v>15</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="M17" s="15">
-        <f>E17</f>
-        <v>16</v>
+        <f t="shared" si="5"/>
+        <v>9</v>
       </c>
       <c r="N17" s="15">
-        <f>L17-M17</f>
-        <v>-1</v>
+        <f t="shared" si="6"/>
+        <v>-3</v>
       </c>
       <c r="O17" s="15">
-        <f>MAX(0,N17)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q17" t="s">
@@ -16814,68 +16808,66 @@
       </c>
       <c r="R17" s="9">
         <f>SUM(M1_Tab2[T])</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T17" s="17" t="str">
         <f>G17</f>
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="U17" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V17" s="35">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="9"/>
+        <v>2</v>
       </c>
       <c r="W17" s="15"/>
       <c r="X17" s="15"/>
     </row>
     <row r="18" spans="2:32">
-      <c r="B18" s="15">
-        <v>4</v>
-      </c>
+      <c r="B18" s="15"/>
       <c r="C18" s="15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D18" s="15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E18" s="15">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="15" t="str">
-        <f>C18</f>
-        <v>C</v>
+        <f t="shared" si="0"/>
+        <v>D</v>
       </c>
       <c r="H18" s="15">
-        <f>IF(ISNUMBER(I17),I17,0)</f>
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="I18" s="15">
-        <f>H18+D18</f>
-        <v>18</v>
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15" t="str">
-        <f>G18</f>
-        <v>C</v>
+        <f t="shared" si="3"/>
+        <v>D</v>
       </c>
       <c r="L18" s="15">
-        <f>I18</f>
-        <v>18</v>
+        <f t="shared" si="4"/>
+        <v>12</v>
       </c>
       <c r="M18" s="15">
-        <f>E18</f>
-        <v>19</v>
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="N18" s="15">
-        <f>L18-M18</f>
-        <v>-1</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="O18" s="15">
-        <f>MAX(0,N18)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q18" t="s">
@@ -16883,154 +16875,111 @@
       </c>
       <c r="R18" s="9">
         <f>MAX(M1_Tab2[T])</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T18" s="17" t="str">
         <f>G18</f>
-        <v>C</v>
+        <v>D</v>
       </c>
       <c r="U18" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V18" s="35">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
     </row>
     <row r="19" spans="2:32">
-      <c r="B19" s="15">
-        <v>5</v>
-      </c>
+      <c r="B19" s="15"/>
       <c r="C19" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E19" s="15">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15" t="str">
-        <f>C19</f>
+        <f t="shared" si="0"/>
         <v>B</v>
       </c>
       <c r="H19" s="15">
-        <f>IF(ISNUMBER(I18),I18,0)</f>
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="I19" s="15">
-        <f>H19+D19</f>
-        <v>20</v>
+        <f t="shared" si="2"/>
+        <v>16</v>
       </c>
       <c r="J19" s="15"/>
       <c r="K19" s="15" t="str">
-        <f>G19</f>
+        <f t="shared" si="3"/>
         <v>B</v>
       </c>
       <c r="L19" s="15">
-        <f>I19</f>
-        <v>20</v>
+        <f t="shared" si="4"/>
+        <v>16</v>
       </c>
       <c r="M19" s="15">
-        <f>E19</f>
-        <v>20</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="N19" s="15">
-        <f>L19-M19</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>8</v>
       </c>
       <c r="O19" s="15">
-        <f>MAX(0,N19)</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="Q19" t="s">
         <v>22</v>
       </c>
       <c r="R19" s="25">
         <f>COUNTIF(M1_Tab2[T],"&gt;0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19" s="17" t="str">
         <f>G19</f>
         <v>B</v>
       </c>
       <c r="U19" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V19" s="35">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" si="9"/>
+        <v>4</v>
       </c>
       <c r="W19" s="15"/>
       <c r="X19" s="15"/>
     </row>
     <row r="20" spans="2:32">
-      <c r="B20" s="18">
-        <v>6</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="18">
-        <v>1</v>
-      </c>
-      <c r="E20" s="18">
-        <v>21</v>
-      </c>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="18" t="str">
-        <f>C20</f>
-        <v>F</v>
-      </c>
-      <c r="H20" s="18">
-        <f>IF(ISNUMBER(I19),I19,0)</f>
-        <v>20</v>
-      </c>
-      <c r="I20" s="18">
-        <f>H20+D20</f>
-        <v>21</v>
-      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
       <c r="J20" s="18"/>
-      <c r="K20" s="18" t="str">
-        <f>G20</f>
-        <v>F</v>
-      </c>
-      <c r="L20" s="18">
-        <f>I20</f>
-        <v>21</v>
-      </c>
-      <c r="M20" s="18">
-        <f>E20</f>
-        <v>21</v>
-      </c>
-      <c r="N20" s="18">
-        <f>L20-M20</f>
-        <v>0</v>
-      </c>
-      <c r="O20" s="18">
-        <f>MAX(0,N20)</f>
-        <v>0</v>
-      </c>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
       <c r="P20" s="15"/>
       <c r="Q20" s="20"/>
       <c r="R20" s="20"/>
-      <c r="T20" s="48" t="str">
-        <f>G20</f>
-        <v>F</v>
-      </c>
-      <c r="U20" s="49">
-        <f>H20</f>
-        <v>20</v>
-      </c>
-      <c r="V20" s="49">
-        <f>I20-H20</f>
-        <v>1</v>
-      </c>
+      <c r="T20" s="44"/>
+      <c r="U20" s="45"/>
+      <c r="V20" s="45"/>
       <c r="W20" s="15"/>
       <c r="X20" s="15"/>
     </row>
@@ -17767,46 +17716,46 @@
       <c r="C26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="45" t="s">
+      <c r="I26" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
       <c r="M26" s="21"/>
-      <c r="N26" s="45" t="s">
+      <c r="N26" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="O26" s="45"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="45"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
       <c r="R26" s="21"/>
-      <c r="S26" s="45" t="s">
+      <c r="S26" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="T26" s="45"/>
-      <c r="U26" s="45"/>
-      <c r="V26" s="45"/>
+      <c r="T26" s="47"/>
+      <c r="U26" s="47"/>
+      <c r="V26" s="47"/>
       <c r="W26" s="21"/>
       <c r="X26" s="21"/>
       <c r="Y26" s="21"/>
-      <c r="AH26" s="44" t="s">
+      <c r="AH26" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="AI26" s="44"/>
-      <c r="AJ26" s="44"/>
+      <c r="AI26" s="46"/>
+      <c r="AJ26" s="46"/>
       <c r="AK26" s="15"/>
-      <c r="AL26" s="44" t="s">
+      <c r="AL26" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="AM26" s="44"/>
-      <c r="AN26" s="44"/>
+      <c r="AM26" s="46"/>
+      <c r="AN26" s="46"/>
       <c r="AO26" s="15"/>
-      <c r="AP26" s="44" t="s">
+      <c r="AP26" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AQ26" s="44"/>
-      <c r="AR26" s="44"/>
+      <c r="AQ26" s="46"/>
+      <c r="AR26" s="46"/>
     </row>
     <row r="27" spans="2:50">
       <c r="B27" s="22"/>
@@ -19675,30 +19624,30 @@
       <c r="B18" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="45" t="s">
+      <c r="H18" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="L18" s="45" t="s">
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="L18" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="47"/>
       <c r="U18" s="15"/>
       <c r="V18" s="15"/>
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
-      <c r="Y18" s="44" t="s">
+      <c r="Y18" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="Z18" s="44"/>
-      <c r="AA18" s="44"/>
-      <c r="AC18" s="44" t="s">
+      <c r="Z18" s="46"/>
+      <c r="AA18" s="46"/>
+      <c r="AC18" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="AD18" s="44"/>
-      <c r="AE18" s="44"/>
+      <c r="AD18" s="46"/>
+      <c r="AE18" s="46"/>
     </row>
     <row r="19" spans="2:31">
       <c r="B19" s="15"/>
@@ -21016,21 +20965,21 @@
       <c r="BJ25" s="38"/>
     </row>
     <row r="26" spans="2:65">
-      <c r="L26" s="46" t="s">
+      <c r="L26" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="M26" s="46"/>
-      <c r="N26" s="46"/>
-      <c r="P26" s="46" t="s">
+      <c r="M26" s="48"/>
+      <c r="N26" s="48"/>
+      <c r="P26" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="46"/>
-      <c r="T26" s="46" t="s">
+      <c r="Q26" s="48"/>
+      <c r="R26" s="48"/>
+      <c r="T26" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="U26" s="46"/>
-      <c r="V26" s="46"/>
+      <c r="U26" s="48"/>
+      <c r="V26" s="48"/>
       <c r="AJ26"/>
       <c r="AK26"/>
       <c r="AL26"/>
@@ -21060,30 +21009,30 @@
       <c r="AM27"/>
       <c r="AN27"/>
       <c r="AO27"/>
-      <c r="AS27" s="46" t="s">
+      <c r="AS27" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="AT27" s="46"/>
-      <c r="AU27" s="46"/>
-      <c r="AV27" s="46"/>
-      <c r="AW27" s="46"/>
-      <c r="AX27" s="46"/>
-      <c r="AZ27" s="46" t="s">
+      <c r="AT27" s="48"/>
+      <c r="AU27" s="48"/>
+      <c r="AV27" s="48"/>
+      <c r="AW27" s="48"/>
+      <c r="AX27" s="48"/>
+      <c r="AZ27" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="BA27" s="46"/>
-      <c r="BB27" s="46"/>
-      <c r="BC27" s="46"/>
-      <c r="BD27" s="46"/>
-      <c r="BE27" s="46"/>
-      <c r="BG27" s="46" t="s">
+      <c r="BA27" s="48"/>
+      <c r="BB27" s="48"/>
+      <c r="BC27" s="48"/>
+      <c r="BD27" s="48"/>
+      <c r="BE27" s="48"/>
+      <c r="BG27" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="BH27" s="46"/>
-      <c r="BI27" s="46"/>
-      <c r="BJ27" s="46"/>
-      <c r="BK27" s="46"/>
-      <c r="BL27" s="46"/>
+      <c r="BH27" s="48"/>
+      <c r="BI27" s="48"/>
+      <c r="BJ27" s="48"/>
+      <c r="BK27" s="48"/>
+      <c r="BL27" s="48"/>
     </row>
     <row r="28" spans="2:65">
       <c r="L28"/>
@@ -23689,21 +23638,21 @@
       <c r="B26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="47" t="s">
+      <c r="I26" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
-      <c r="M26" s="47" t="s">
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="M26" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="N26" s="47"/>
-      <c r="O26" s="47"/>
-      <c r="Q26" s="47" t="s">
+      <c r="N26" s="49"/>
+      <c r="O26" s="49"/>
+      <c r="Q26" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="R26" s="47"/>
-      <c r="S26" s="47"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="49"/>
       <c r="U26" s="21"/>
       <c r="V26" s="21"/>
       <c r="W26" s="21"/>
@@ -23713,22 +23662,22 @@
       <c r="AA26" s="21"/>
       <c r="AB26" s="21"/>
       <c r="AC26" s="21"/>
-      <c r="AD26" s="44" t="s">
+      <c r="AD26" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="AE26" s="44"/>
-      <c r="AF26" s="44"/>
+      <c r="AE26" s="46"/>
+      <c r="AF26" s="46"/>
       <c r="AG26" s="15"/>
-      <c r="AH26" s="44" t="s">
+      <c r="AH26" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="AI26" s="44"/>
-      <c r="AJ26" s="44"/>
-      <c r="AL26" s="44" t="s">
+      <c r="AI26" s="46"/>
+      <c r="AJ26" s="46"/>
+      <c r="AL26" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="AM26" s="44"/>
-      <c r="AN26" s="44"/>
+      <c r="AM26" s="46"/>
+      <c r="AN26" s="46"/>
     </row>
     <row r="27" spans="2:40">
       <c r="B27" s="15"/>

</xml_diff>

<commit_message>
FINALIZADO Tarefa 2 - Aula 2
</commit_message>
<xml_diff>
--- a/Aula 1/3515 L01 Sched 2020.xlsx
+++ b/Aula 1/3515 L01 Sched 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thale\Documents\Faculdade\PRO3515 - Algoritmos de Otimização para Problemas de Programação da Produção\Aula 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4B6F24-5D21-4AC0-9B38-90AFCCA96A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2298F6-A52C-4B95-8D37-3A5FC2F6E4FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16371,7 +16371,7 @@
   <dimension ref="A1:AF27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -16637,36 +16637,36 @@
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15" t="str">
-        <f t="shared" ref="G15:G20" si="0">C15</f>
+        <f t="shared" ref="G15:G19" si="0">C15</f>
         <v>E</v>
       </c>
       <c r="H15" s="15">
-        <f t="shared" ref="H15:H20" si="1">IF(ISNUMBER(I14),I14,0)</f>
+        <f t="shared" ref="H15:H19" si="1">IF(ISNUMBER(I14),I14,0)</f>
         <v>0</v>
       </c>
       <c r="I15" s="15">
-        <f t="shared" ref="I15:I20" si="2">H15+D15</f>
+        <f t="shared" ref="I15:I19" si="2">H15+D15</f>
         <v>1</v>
       </c>
       <c r="J15" s="15"/>
       <c r="K15" s="15" t="str">
-        <f t="shared" ref="K15:K20" si="3">G15</f>
+        <f t="shared" ref="K15:K19" si="3">G15</f>
         <v>E</v>
       </c>
       <c r="L15" s="15">
-        <f t="shared" ref="L15:L20" si="4">I15</f>
+        <f t="shared" ref="L15:L19" si="4">I15</f>
         <v>1</v>
       </c>
       <c r="M15" s="15">
-        <f t="shared" ref="M15:M20" si="5">E15</f>
+        <f t="shared" ref="M15:M19" si="5">E15</f>
         <v>4</v>
       </c>
       <c r="N15" s="15">
-        <f t="shared" ref="N15:N20" si="6">L15-M15</f>
+        <f t="shared" ref="N15:N19" si="6">L15-M15</f>
         <v>-3</v>
       </c>
       <c r="O15" s="15">
-        <f t="shared" ref="O15:O20" si="7">MAX(0,N15)</f>
+        <f t="shared" ref="O15:O19" si="7">MAX(0,N15)</f>
         <v>0</v>
       </c>
       <c r="Q15" t="s">

</xml_diff>

<commit_message>
Aula 3 - ex 1
</commit_message>
<xml_diff>
--- a/Aula 1/3515 L01 Sched 2020.xlsx
+++ b/Aula 1/3515 L01 Sched 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thale\Documents\Faculdade\PRO3515 - Algoritmos de Otimização para Problemas de Programação da Produção\Aula 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2298F6-A52C-4B95-8D37-3A5FC2F6E4FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3311FB86-A520-48CB-8F83-1F3434830B61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M1" sheetId="30" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="48">
   <si>
     <t>#</t>
   </si>
@@ -160,18 +160,6 @@
     <t>M3</t>
   </si>
   <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
     <t>Flow Shop Scheduling</t>
   </si>
   <si>
@@ -227,7 +215,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -335,10 +323,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -363,7 +347,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -444,10 +428,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -462,6 +443,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1661,7 +1647,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>E</c:v>
+                  <c:v>A</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1718,7 +1704,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1777,7 +1763,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A</c:v>
+                  <c:v>B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1834,7 +1820,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1950,7 +1936,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2066,7 +2052,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2125,7 +2111,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B</c:v>
+                  <c:v>E</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2182,7 +2168,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4437,7 +4423,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A</c:v>
+                  <c:v>E</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4494,7 +4480,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4553,7 +4539,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B</c:v>
+                  <c:v>D</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4610,7 +4596,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4669,7 +4655,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C</c:v>
+                  <c:v>A</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4726,7 +4712,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5710,7 +5696,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>D</c:v>
+                  <c:v>F</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5767,7 +5753,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5826,7 +5812,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>E</c:v>
+                  <c:v>C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5883,7 +5869,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5941,6 +5927,9 @@
               <c:f>'MP3'!$AL$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>B</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -5996,7 +5985,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6979,9 +6968,6 @@
               <c:f>'MP3'!$AP$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>F</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -7037,7 +7023,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7095,9 +7081,6 @@
               <c:f>'MP3'!$AP$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>G</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -7153,7 +7136,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7211,9 +7194,6 @@
               <c:f>'MP3'!$AP$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>H</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -7269,7 +7249,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7327,9 +7307,6 @@
               <c:f>'MP3'!$AP$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>I</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -7385,7 +7362,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7443,9 +7420,6 @@
               <c:f>'MP3'!$AP$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>J</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -7501,7 +7475,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15253,10 +15227,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="M1_Tab0" displayName="M1_Tab0" ref="B14:E19" totalsRowShown="0" headerRowDxfId="115">
-  <autoFilter ref="B14:E19" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B15:E19">
-    <sortCondition ref="B14:B19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="M1_Tab0" displayName="M1_Tab0" ref="B14:E20" totalsRowShown="0" headerRowDxfId="115">
+  <autoFilter ref="B14:E20" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B15:E20">
+    <sortCondition ref="C14:C20"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#"/>
@@ -15287,8 +15261,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="MP3_TabM3" displayName="MP3_TabM3" ref="S28:V38" totalsRowShown="0" headerRowDxfId="83">
-  <autoFilter ref="S28:V38" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="MP3_TabM3" displayName="MP3_TabM3" ref="S28:V36" totalsRowShown="0" headerRowDxfId="83">
+  <autoFilter ref="S28:V36" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="4">
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="Op"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Job" dataDxfId="82">
@@ -15442,8 +15416,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="M1_Tab1" displayName="M1_Tab1" ref="G14:I19" totalsRowShown="0" headerRowDxfId="114">
-  <autoFilter ref="G14:I19" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="M1_Tab1" displayName="M1_Tab1" ref="G14:I20" totalsRowShown="0" headerRowDxfId="114">
+  <autoFilter ref="G14:I20" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Job">
       <calculatedColumnFormula>C15</calculatedColumnFormula>
@@ -15642,8 +15616,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="M1_Tab2" displayName="M1_Tab2" ref="K14:O19" totalsRowShown="0" headerRowDxfId="113">
-  <autoFilter ref="K14:O19" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="M1_Tab2" displayName="M1_Tab2" ref="K14:O20" totalsRowShown="0" headerRowDxfId="113">
+  <autoFilter ref="K14:O20" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K17:O21">
     <sortCondition ref="K15:K20"/>
   </sortState>
@@ -15867,8 +15841,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="M1_Tab4" displayName="M1_Tab4" ref="T14:V19" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
-  <autoFilter ref="T14:V19" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="M1_Tab4" displayName="M1_Tab4" ref="T14:V20" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
+  <autoFilter ref="T14:V20" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Job" dataDxfId="110">
       <calculatedColumnFormula>G15</calculatedColumnFormula>
@@ -15930,10 +15904,10 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="MP3_Tab0" displayName="MP3_Tab0" ref="B28:G38" totalsRowShown="0" headerRowDxfId="105">
-  <autoFilter ref="B28:G38" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B29:G38">
-    <sortCondition ref="E28:E38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="MP3_Tab0" displayName="MP3_Tab0" ref="B28:G34" totalsRowShown="0" headerRowDxfId="105">
+  <autoFilter ref="B28:G34" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B29:G34">
+    <sortCondition ref="C28:C34"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="m" dataDxfId="104" dataCellStyle="Normal 3"/>
@@ -15950,8 +15924,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="MP3_TabM1" displayName="MP3_TabM1" ref="I28:L38" totalsRowShown="0" headerRowDxfId="101">
-  <autoFilter ref="I28:L38" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="MP3_TabM1" displayName="MP3_TabM1" ref="I28:L36" totalsRowShown="0" headerRowDxfId="101">
+  <autoFilter ref="I28:L36" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="4">
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Op"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Job" dataDxfId="100">
@@ -15969,8 +15943,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="MP3_TabM2" displayName="MP3_TabM2" ref="N28:Q38" totalsRowShown="0" headerRowDxfId="98">
-  <autoFilter ref="N28:Q38" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="MP3_TabM2" displayName="MP3_TabM2" ref="N28:Q36" totalsRowShown="0" headerRowDxfId="98">
+  <autoFilter ref="N28:Q36" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="4">
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Op"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Job" dataDxfId="97">
@@ -15988,8 +15962,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="MP3_Tab2" displayName="MP3_Tab2" ref="X28:AC38" totalsRowShown="0" headerRowDxfId="95">
-  <autoFilter ref="X28:AC38" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="MP3_Tab2" displayName="MP3_Tab2" ref="X28:AC34" totalsRowShown="0" headerRowDxfId="95">
+  <autoFilter ref="X28:AC34" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="X29:AC38">
     <sortCondition ref="Y26:Y36"/>
   </sortState>
@@ -16370,11 +16344,11 @@
   </sheetPr>
   <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="16" width="5.6328125" style="13" customWidth="1"/>
     <col min="17" max="17" width="20.6328125" style="13" customWidth="1"/>
@@ -16382,7 +16356,7 @@
     <col min="27" max="16384" width="8.90625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="12" customFormat="1" ht="26">
+    <row r="1" spans="1:32" s="12" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="10" t="s">
         <v>26</v>
       </c>
@@ -16405,7 +16379,7 @@
       <c r="R1" s="10"/>
       <c r="S1" s="10"/>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -16424,12 +16398,12 @@
       <c r="Q2" s="14"/>
       <c r="R2" s="14"/>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -16443,7 +16417,7 @@
       <c r="Z4" s="15"/>
       <c r="AA4" s="15"/>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -16457,7 +16431,7 @@
       <c r="Z5" s="15"/>
       <c r="AA5" s="15"/>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -16471,28 +16445,28 @@
       <c r="Z6" s="15"/>
       <c r="AA6" s="15"/>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="T10" s="15"/>
       <c r="U10" s="15"/>
       <c r="V10" s="15"/>
@@ -16507,7 +16481,7 @@
       <c r="AE10" s="15"/>
       <c r="AF10" s="15"/>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
@@ -16523,7 +16497,7 @@
       <c r="AE11" s="15"/>
       <c r="AF11" s="15"/>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B12" s="16" t="s">
         <v>24</v>
       </c>
@@ -16533,11 +16507,11 @@
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
       <c r="S12" s="15"/>
-      <c r="T12" s="46" t="s">
+      <c r="T12" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="U12" s="46"/>
-      <c r="V12" s="46"/>
+      <c r="U12" s="45"/>
+      <c r="V12" s="45"/>
       <c r="W12" s="15"/>
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
@@ -16546,7 +16520,7 @@
       <c r="AB12" s="15"/>
       <c r="AC12" s="15"/>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B13" s="15"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -16571,7 +16545,7 @@
       <c r="AB13" s="15"/>
       <c r="AC13" s="15"/>
     </row>
-    <row r="14" spans="1:32" customFormat="1" ht="13">
+    <row r="14" spans="1:32" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="B14" s="41" t="s">
         <v>0</v>
       </c>
@@ -16609,7 +16583,7 @@
         <v>11</v>
       </c>
       <c r="Q14" s="41" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="R14" s="41" t="s">
         <v>25</v>
@@ -16621,24 +16595,24 @@
         <v>14</v>
       </c>
       <c r="V14" s="41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B15" s="15"/>
       <c r="C15" s="15" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D15" s="15">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E15" s="15">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15" t="str">
         <f t="shared" ref="G15:G19" si="0">C15</f>
-        <v>E</v>
+        <v>A</v>
       </c>
       <c r="H15" s="15">
         <f t="shared" ref="H15:H19" si="1">IF(ISNUMBER(I14),I14,0)</f>
@@ -16646,24 +16620,24 @@
       </c>
       <c r="I15" s="15">
         <f t="shared" ref="I15:I19" si="2">H15+D15</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J15" s="15"/>
       <c r="K15" s="15" t="str">
         <f t="shared" ref="K15:K19" si="3">G15</f>
-        <v>E</v>
+        <v>A</v>
       </c>
       <c r="L15" s="15">
         <f t="shared" ref="L15:L19" si="4">I15</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M15" s="15">
         <f t="shared" ref="M15:M19" si="5">E15</f>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="N15" s="15">
         <f t="shared" ref="N15:N19" si="6">L15-M15</f>
-        <v>-3</v>
+        <v>-14</v>
       </c>
       <c r="O15" s="15">
         <f t="shared" ref="O15:O19" si="7">MAX(0,N15)</f>
@@ -16674,11 +16648,11 @@
       </c>
       <c r="R15" s="9">
         <f>MAX(M1_Tab2[C])</f>
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="T15" s="17" t="str">
         <f>G15</f>
-        <v>E</v>
+        <v>A</v>
       </c>
       <c r="U15" s="35">
         <f>H15</f>
@@ -16686,51 +16660,51 @@
       </c>
       <c r="V15" s="35">
         <f>I15-H15</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="W15" s="15"/>
       <c r="X15" s="15"/>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B16" s="15"/>
       <c r="C16" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16" s="15">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E16" s="15">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="H16" s="15">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I16" s="15">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="L16" s="15">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="M16" s="15">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="N16" s="15">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="O16" s="15">
         <f t="shared" si="7"/>
@@ -16741,11 +16715,11 @@
       </c>
       <c r="R16" s="9">
         <f>AVERAGE(M1_Tab2[C])</f>
-        <v>7.8</v>
+        <v>30.833333333333332</v>
       </c>
       <c r="T16" s="17" t="str">
         <f>G16</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="U16" s="35">
         <f t="shared" ref="U16:U19" si="8">H16-I15</f>
@@ -16753,21 +16727,21 @@
       </c>
       <c r="V16" s="35">
         <f t="shared" ref="V16:V19" si="9">I16-H16</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="W16" s="15"/>
       <c r="X16" s="15"/>
     </row>
-    <row r="17" spans="2:32">
+    <row r="17" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B17" s="15"/>
       <c r="C17" s="15" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="15">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E17" s="15">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15" t="str">
@@ -16776,11 +16750,11 @@
       </c>
       <c r="H17" s="15">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="I17" s="15">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15" t="str">
@@ -16789,26 +16763,26 @@
       </c>
       <c r="L17" s="15">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="M17" s="15">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="N17" s="15">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="O17" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17" t="s">
         <v>20</v>
       </c>
       <c r="R17" s="9">
         <f>SUM(M1_Tab2[T])</f>
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="T17" s="17" t="str">
         <f>G17</f>
@@ -16820,21 +16794,21 @@
       </c>
       <c r="V17" s="35">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="W17" s="15"/>
       <c r="X17" s="15"/>
     </row>
-    <row r="18" spans="2:32">
+    <row r="18" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B18" s="15"/>
       <c r="C18" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="15">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E18" s="15">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="15" t="str">
@@ -16843,11 +16817,11 @@
       </c>
       <c r="H18" s="15">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="I18" s="15">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15" t="str">
@@ -16856,26 +16830,26 @@
       </c>
       <c r="L18" s="15">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="M18" s="15">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="N18" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O18" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Q18" t="s">
         <v>21</v>
       </c>
       <c r="R18" s="9">
         <f>MAX(M1_Tab2[T])</f>
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="T18" s="17" t="str">
         <f>G18</f>
@@ -16887,66 +16861,66 @@
       </c>
       <c r="V18" s="35">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
     </row>
-    <row r="19" spans="2:32">
+    <row r="19" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B19" s="15"/>
       <c r="C19" s="15" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D19" s="15">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E19" s="15">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>B</v>
+        <v>E</v>
       </c>
       <c r="H19" s="15">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="I19" s="15">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J19" s="15"/>
       <c r="K19" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>B</v>
+        <v>E</v>
       </c>
       <c r="L19" s="15">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="M19" s="15">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="N19" s="15">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="O19" s="15">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="Q19" t="s">
         <v>22</v>
       </c>
       <c r="R19" s="25">
         <f>COUNTIF(M1_Tab2[T],"&gt;0")</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T19" s="17" t="str">
         <f>G19</f>
-        <v>B</v>
+        <v>E</v>
       </c>
       <c r="U19" s="35">
         <f t="shared" si="8"/>
@@ -16954,36 +16928,75 @@
       </c>
       <c r="V19" s="35">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="W19" s="15"/>
       <c r="X19" s="15"/>
     </row>
-    <row r="20" spans="2:32">
+    <row r="20" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+      <c r="C20" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="18">
+        <v>15</v>
+      </c>
+      <c r="E20" s="15">
+        <v>20</v>
+      </c>
       <c r="F20" s="15"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="G20" s="18" t="str">
+        <f>C20</f>
+        <v>F</v>
+      </c>
+      <c r="H20" s="18">
+        <f>IF(ISNUMBER(I19),I19,0)</f>
+        <v>48</v>
+      </c>
+      <c r="I20" s="18">
+        <f>H20+D20</f>
+        <v>63</v>
+      </c>
       <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
+      <c r="K20" s="18" t="str">
+        <f>G20</f>
+        <v>F</v>
+      </c>
+      <c r="L20" s="18">
+        <f>I20</f>
+        <v>63</v>
+      </c>
+      <c r="M20" s="18">
+        <f>E20</f>
+        <v>20</v>
+      </c>
+      <c r="N20" s="18">
+        <f>L20-M20</f>
+        <v>43</v>
+      </c>
+      <c r="O20" s="18">
+        <f>MAX(0,N20)</f>
+        <v>43</v>
+      </c>
       <c r="P20" s="15"/>
       <c r="Q20" s="20"/>
       <c r="R20" s="20"/>
-      <c r="T20" s="44"/>
-      <c r="U20" s="45"/>
-      <c r="V20" s="45"/>
+      <c r="T20" s="44" t="str">
+        <f>G20</f>
+        <v>F</v>
+      </c>
+      <c r="U20" s="49">
+        <f>H20</f>
+        <v>48</v>
+      </c>
+      <c r="V20" s="49">
+        <f>I20-H20</f>
+        <v>15</v>
+      </c>
       <c r="W20" s="15"/>
       <c r="X20" s="15"/>
     </row>
-    <row r="21" spans="2:32">
+    <row r="21" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -17007,7 +17020,7 @@
       <c r="W21" s="15"/>
       <c r="X21" s="15"/>
     </row>
-    <row r="22" spans="2:32">
+    <row r="22" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -17036,7 +17049,7 @@
       <c r="AB22" s="15"/>
       <c r="AC22" s="15"/>
     </row>
-    <row r="23" spans="2:32">
+    <row r="23" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -17065,7 +17078,7 @@
       <c r="AB23" s="15"/>
       <c r="AC23" s="15"/>
     </row>
-    <row r="24" spans="2:32">
+    <row r="24" spans="2:32" x14ac:dyDescent="0.35">
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
@@ -17094,7 +17107,7 @@
       <c r="AB24" s="15"/>
       <c r="AC24" s="15"/>
     </row>
-    <row r="25" spans="2:32">
+    <row r="25" spans="2:32" x14ac:dyDescent="0.35">
       <c r="T25" s="15"/>
       <c r="U25" s="15"/>
       <c r="V25" s="15"/>
@@ -17106,7 +17119,7 @@
       <c r="AB25" s="15"/>
       <c r="AC25" s="15"/>
     </row>
-    <row r="26" spans="2:32">
+    <row r="26" spans="2:32" x14ac:dyDescent="0.35">
       <c r="T26" s="15"/>
       <c r="U26" s="15"/>
       <c r="V26" s="15"/>
@@ -17121,7 +17134,7 @@
       <c r="AE26" s="15"/>
       <c r="AF26" s="15"/>
     </row>
-    <row r="27" spans="2:32">
+    <row r="27" spans="2:32" x14ac:dyDescent="0.35">
       <c r="T27" s="15"/>
       <c r="U27" s="15"/>
       <c r="V27" s="15"/>
@@ -17167,11 +17180,11 @@
   </sheetPr>
   <dimension ref="A1:AX47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="30" width="5.6328125" style="13" customWidth="1"/>
     <col min="31" max="31" width="20.6328125" style="13" customWidth="1"/>
@@ -17179,7 +17192,7 @@
     <col min="45" max="16384" width="8.90625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="12" customFormat="1" ht="26">
+    <row r="1" spans="1:50" s="12" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="10" t="s">
         <v>28</v>
       </c>
@@ -17207,7 +17220,7 @@
       <c r="W1" s="10"/>
       <c r="X1" s="10"/>
     </row>
-    <row r="3" spans="1:50">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
       <c r="Z3"/>
       <c r="AA3"/>
       <c r="AB3"/>
@@ -17220,7 +17233,7 @@
       <c r="AI3"/>
       <c r="AJ3"/>
     </row>
-    <row r="4" spans="1:50">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -17242,7 +17255,7 @@
       <c r="AT4" s="15"/>
       <c r="AU4" s="15"/>
     </row>
-    <row r="5" spans="1:50">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -17264,7 +17277,7 @@
       <c r="AT5" s="15"/>
       <c r="AU5" s="15"/>
     </row>
-    <row r="6" spans="1:50">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -17286,7 +17299,7 @@
       <c r="AT6" s="15"/>
       <c r="AU6" s="15"/>
     </row>
-    <row r="7" spans="1:50">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -17300,7 +17313,7 @@
       <c r="AG7" s="9"/>
       <c r="AJ7"/>
     </row>
-    <row r="8" spans="1:50">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -17314,7 +17327,7 @@
       <c r="AG8" s="9"/>
       <c r="AJ8"/>
     </row>
-    <row r="9" spans="1:50">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -17328,7 +17341,7 @@
       <c r="AG9" s="25"/>
       <c r="AJ9"/>
     </row>
-    <row r="10" spans="1:50">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -17347,7 +17360,7 @@
       <c r="AP10" s="15"/>
       <c r="AQ10" s="15"/>
     </row>
-    <row r="11" spans="1:50">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -17376,7 +17389,7 @@
       <c r="AW11" s="15"/>
       <c r="AX11" s="15"/>
     </row>
-    <row r="12" spans="1:50">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -17398,7 +17411,7 @@
       <c r="AW12" s="15"/>
       <c r="AX12" s="15"/>
     </row>
-    <row r="13" spans="1:50">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -17420,7 +17433,7 @@
       <c r="AW13" s="15"/>
       <c r="AX13" s="15"/>
     </row>
-    <row r="14" spans="1:50">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -17435,7 +17448,7 @@
       <c r="AP14" s="15"/>
       <c r="AQ14" s="15"/>
     </row>
-    <row r="15" spans="1:50">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -17450,7 +17463,7 @@
       <c r="AP15" s="15"/>
       <c r="AQ15" s="15"/>
     </row>
-    <row r="16" spans="1:50">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.35">
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
@@ -17472,7 +17485,7 @@
       <c r="AP16" s="15"/>
       <c r="AQ16" s="15"/>
     </row>
-    <row r="17" spans="2:50">
+    <row r="17" spans="2:50" x14ac:dyDescent="0.35">
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -17496,7 +17509,7 @@
       <c r="AP17" s="15"/>
       <c r="AQ17" s="15"/>
     </row>
-    <row r="18" spans="2:50">
+    <row r="18" spans="2:50" x14ac:dyDescent="0.35">
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -17527,7 +17540,7 @@
       <c r="AW18" s="15"/>
       <c r="AX18" s="15"/>
     </row>
-    <row r="19" spans="2:50">
+    <row r="19" spans="2:50" x14ac:dyDescent="0.35">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -17558,7 +17571,7 @@
       <c r="AW19" s="15"/>
       <c r="AX19" s="15"/>
     </row>
-    <row r="20" spans="2:50">
+    <row r="20" spans="2:50" x14ac:dyDescent="0.35">
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -17589,7 +17602,7 @@
       <c r="AW20" s="15"/>
       <c r="AX20" s="15"/>
     </row>
-    <row r="21" spans="2:50">
+    <row r="21" spans="2:50" x14ac:dyDescent="0.35">
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
@@ -17613,7 +17626,7 @@
       <c r="AP21" s="15"/>
       <c r="AQ21" s="15"/>
     </row>
-    <row r="22" spans="2:50">
+    <row r="22" spans="2:50" x14ac:dyDescent="0.35">
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
@@ -17637,7 +17650,7 @@
       <c r="AP22" s="15"/>
       <c r="AQ22" s="15"/>
     </row>
-    <row r="23" spans="2:50">
+    <row r="23" spans="2:50" x14ac:dyDescent="0.35">
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
@@ -17661,7 +17674,7 @@
       <c r="AP23" s="15"/>
       <c r="AQ23" s="15"/>
     </row>
-    <row r="24" spans="2:50">
+    <row r="24" spans="2:50" x14ac:dyDescent="0.35">
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
@@ -17685,7 +17698,7 @@
       <c r="AP24" s="15"/>
       <c r="AQ24" s="15"/>
     </row>
-    <row r="25" spans="2:50">
+    <row r="25" spans="2:50" x14ac:dyDescent="0.35">
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
@@ -17709,55 +17722,55 @@
       <c r="AP25" s="15"/>
       <c r="AQ25" s="15"/>
     </row>
-    <row r="26" spans="2:50">
+    <row r="26" spans="2:50" x14ac:dyDescent="0.35">
       <c r="B26" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="47" t="s">
+      <c r="I26" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="47"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
       <c r="M26" s="21"/>
-      <c r="N26" s="47" t="s">
+      <c r="N26" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="O26" s="47"/>
-      <c r="P26" s="47"/>
-      <c r="Q26" s="47"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="46"/>
+      <c r="Q26" s="46"/>
       <c r="R26" s="21"/>
-      <c r="S26" s="47" t="s">
+      <c r="S26" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="T26" s="47"/>
-      <c r="U26" s="47"/>
-      <c r="V26" s="47"/>
+      <c r="T26" s="46"/>
+      <c r="U26" s="46"/>
+      <c r="V26" s="46"/>
       <c r="W26" s="21"/>
       <c r="X26" s="21"/>
       <c r="Y26" s="21"/>
-      <c r="AH26" s="46" t="s">
+      <c r="AH26" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="AI26" s="46"/>
-      <c r="AJ26" s="46"/>
+      <c r="AI26" s="45"/>
+      <c r="AJ26" s="45"/>
       <c r="AK26" s="15"/>
-      <c r="AL26" s="46" t="s">
+      <c r="AL26" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="AM26" s="46"/>
-      <c r="AN26" s="46"/>
+      <c r="AM26" s="45"/>
+      <c r="AN26" s="45"/>
       <c r="AO26" s="15"/>
-      <c r="AP26" s="46" t="s">
+      <c r="AP26" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="AQ26" s="46"/>
-      <c r="AR26" s="46"/>
+      <c r="AQ26" s="45"/>
+      <c r="AR26" s="45"/>
     </row>
-    <row r="27" spans="2:50">
+    <row r="27" spans="2:50" x14ac:dyDescent="0.35">
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
       <c r="D27" s="17"/>
@@ -17787,7 +17800,7 @@
       <c r="AQ27" s="15"/>
       <c r="AR27" s="15"/>
     </row>
-    <row r="28" spans="2:50" customFormat="1" ht="13">
+    <row r="28" spans="2:50" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="B28" s="41" t="s">
         <v>29</v>
       </c>
@@ -17861,7 +17874,7 @@
         <v>11</v>
       </c>
       <c r="AE28" s="41" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AF28" s="41" t="s">
         <v>25</v>
@@ -17873,7 +17886,7 @@
         <v>14</v>
       </c>
       <c r="AJ28" s="41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AL28" s="41" t="s">
         <v>1</v>
@@ -17882,7 +17895,7 @@
         <v>14</v>
       </c>
       <c r="AN28" s="41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AP28" s="41" t="s">
         <v>1</v>
@@ -17891,25 +17904,25 @@
         <v>14</v>
       </c>
       <c r="AR28" s="41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="29" spans="2:50">
-      <c r="B29" s="13">
+    <row r="29" spans="2:50" x14ac:dyDescent="0.35">
+      <c r="B29" s="15">
         <v>1</v>
       </c>
       <c r="C29" s="13">
         <v>1</v>
       </c>
       <c r="D29" s="15">
-        <f t="shared" ref="D29:D38" si="0">B29*100+C29</f>
+        <f>B29*100+C29</f>
         <v>101</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F29" s="15">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G29" s="15">
         <v>20</v>
@@ -17920,7 +17933,7 @@
       </c>
       <c r="J29" s="15" t="str">
         <f>IF(ISERROR(VLOOKUP(I29,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(I29,MP3_Tab0[[Op]:[Job]],2,0))</f>
-        <v>A</v>
+        <v>E</v>
       </c>
       <c r="K29" s="15">
         <f>IF(J29="","",IF(ISNUMBER(L28),L28,0))</f>
@@ -17928,7 +17941,7 @@
       </c>
       <c r="L29" s="15">
         <f>IF(J29="","",K29+VLOOKUP(I29,MP3_Tab0[[Op]:[p]],3,0))</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="M29" s="15"/>
       <c r="N29" s="15">
@@ -17936,7 +17949,7 @@
       </c>
       <c r="O29" s="15" t="str">
         <f>IF(ISERROR(VLOOKUP(N29,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(N29,MP3_Tab0[[Op]:[Job]],2,0))</f>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="P29" s="15">
         <f>IF(O29="","",IF(ISNUMBER(Q28),Q28,0))</f>
@@ -17944,7 +17957,7 @@
       </c>
       <c r="Q29" s="15">
         <f>IF(O29="","",P29+VLOOKUP(N29,MP3_Tab0[[Op]:[p]],3,0))</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="R29" s="15"/>
       <c r="S29" s="15">
@@ -17952,39 +17965,39 @@
       </c>
       <c r="T29" s="15" t="str">
         <f>IF(ISERROR(VLOOKUP(S29,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(S29,MP3_Tab0[[Op]:[Job]],2,0))</f>
-        <v>F</v>
-      </c>
-      <c r="U29" s="15">
+        <v/>
+      </c>
+      <c r="U29" s="15" t="str">
         <f>IF(T29="","",IF(ISNUMBER(V28),V28,0))</f>
-        <v>0</v>
-      </c>
-      <c r="V29" s="15">
+        <v/>
+      </c>
+      <c r="V29" s="15" t="str">
         <f>IF(T29="","",U29+VLOOKUP(S29,MP3_Tab0[[Op]:[p]],3,0))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="W29" s="15"/>
       <c r="X29" s="15">
-        <f t="shared" ref="X29:X38" si="1">D29</f>
+        <f t="shared" ref="X29:X38" si="0">D29</f>
         <v>101</v>
       </c>
       <c r="Y29" s="15" t="str">
         <f>VLOOKUP(X29,MP3_Tab0[[Op]:[Job]],2,0)</f>
-        <v>A</v>
+        <v>E</v>
       </c>
       <c r="Z29" s="15" cm="1">
         <f t="array" aca="1" ref="Z29" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B29),C29,4)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="AA29" s="15">
-        <f t="shared" ref="AA29:AA38" si="2">G29</f>
+        <f t="shared" ref="AA29:AA38" si="1">G29</f>
         <v>20</v>
       </c>
       <c r="AB29" s="15">
-        <f t="shared" ref="AB29:AB38" ca="1" si="3">Z29-AA29</f>
-        <v>-16</v>
+        <f t="shared" ref="AB29:AB38" ca="1" si="2">Z29-AA29</f>
+        <v>-6</v>
       </c>
       <c r="AC29" s="15">
-        <f t="shared" ref="AC29:AC38" ca="1" si="4">MAX(0,AB29)</f>
+        <f t="shared" ref="AC29:AC38" ca="1" si="3">MAX(0,AB29)</f>
         <v>0</v>
       </c>
       <c r="AD29" s="15"/>
@@ -17993,24 +18006,24 @@
       </c>
       <c r="AF29" s="9">
         <f ca="1">MAX(MP3_Tab2[C])</f>
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="AG29" s="15"/>
       <c r="AH29" s="17" t="str">
         <f>IF(J29="","",J29)</f>
-        <v>A</v>
+        <v>E</v>
       </c>
       <c r="AI29" s="37">
         <f>IF(K29="","",K29)</f>
         <v>0</v>
       </c>
       <c r="AJ29" s="37">
-        <f t="shared" ref="AJ29:AJ38" si="5">IF(L29="","",L29-K29)</f>
-        <v>4</v>
+        <f t="shared" ref="AJ29:AJ38" si="4">IF(L29="","",L29-K29)</f>
+        <v>14</v>
       </c>
       <c r="AL29" s="37" t="str">
-        <f t="shared" ref="AL29:AL38" si="6">IF(O29="","",O29)</f>
-        <v>D</v>
+        <f t="shared" ref="AL29:AL38" si="5">IF(O29="","",O29)</f>
+        <v>F</v>
       </c>
       <c r="AM29" s="37">
         <f>IF(P29="","",P29)</f>
@@ -18018,39 +18031,39 @@
       </c>
       <c r="AN29" s="37">
         <f>IF(Q29="","",Q29-P29)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AP29" s="37" t="str">
-        <f t="shared" ref="AP29:AP38" si="7">IF(T29="","",T29)</f>
-        <v>F</v>
-      </c>
-      <c r="AQ29" s="37">
+        <f t="shared" ref="AP29:AP38" si="6">IF(T29="","",T29)</f>
+        <v/>
+      </c>
+      <c r="AQ29" s="37" t="str">
         <f>IF(U29="","",U29)</f>
-        <v>0</v>
-      </c>
-      <c r="AR29" s="37">
-        <f t="shared" ref="AR29:AR38" si="8">IF(V29="","",V29-U29)</f>
+        <v/>
+      </c>
+      <c r="AR29" s="37" t="str">
+        <f t="shared" ref="AR29:AR38" si="7">IF(V29="","",V29-U29)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="2:50" x14ac:dyDescent="0.35">
+      <c r="B30" s="15">
+        <v>2</v>
+      </c>
+      <c r="C30" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:50">
-      <c r="B30" s="13">
-        <v>1</v>
-      </c>
-      <c r="C30" s="13">
-        <v>2</v>
-      </c>
       <c r="D30" s="15">
-        <f t="shared" si="0"/>
-        <v>102</v>
+        <f>B30*100+C30</f>
+        <v>201</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F30" s="15">
-        <v>2</v>
-      </c>
-      <c r="G30" s="15">
+        <v>15</v>
+      </c>
+      <c r="G30" s="13">
         <v>20</v>
       </c>
       <c r="H30" s="15"/>
@@ -18059,15 +18072,15 @@
       </c>
       <c r="J30" s="15" t="str">
         <f>IF(ISERROR(VLOOKUP(I30,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(I30,MP3_Tab0[[Op]:[Job]],2,0))</f>
-        <v>B</v>
+        <v>D</v>
       </c>
       <c r="K30" s="15">
         <f>IF(J30="","",IF(ISNUMBER(L29),L29,0))</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="L30" s="15">
         <f>IF(J30="","",K30+VLOOKUP(I30,MP3_Tab0[[Op]:[p]],3,0))</f>
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="M30" s="15"/>
       <c r="N30" s="15">
@@ -18075,15 +18088,15 @@
       </c>
       <c r="O30" s="15" t="str">
         <f>IF(ISERROR(VLOOKUP(N30,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(N30,MP3_Tab0[[Op]:[Job]],2,0))</f>
-        <v>E</v>
+        <v>C</v>
       </c>
       <c r="P30" s="15">
         <f>IF(O30="","",IF(ISNUMBER(Q29),Q29,0))</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Q30" s="15">
         <f>IF(O30="","",P30+VLOOKUP(N30,MP3_Tab0[[Op]:[p]],3,0))</f>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="R30" s="15"/>
       <c r="S30" s="15">
@@ -18091,39 +18104,39 @@
       </c>
       <c r="T30" s="15" t="str">
         <f>IF(ISERROR(VLOOKUP(S30,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(S30,MP3_Tab0[[Op]:[Job]],2,0))</f>
-        <v>G</v>
-      </c>
-      <c r="U30" s="15">
+        <v/>
+      </c>
+      <c r="U30" s="15" t="str">
         <f>IF(T30="","",IF(ISNUMBER(V29),V29,0))</f>
-        <v>1</v>
-      </c>
-      <c r="V30" s="15">
+        <v/>
+      </c>
+      <c r="V30" s="15" t="str">
         <f>IF(T30="","",U30+VLOOKUP(S30,MP3_Tab0[[Op]:[p]],3,0))</f>
-        <v>6</v>
+        <v/>
       </c>
       <c r="W30" s="15"/>
       <c r="X30" s="15">
-        <f t="shared" si="1"/>
-        <v>102</v>
+        <f t="shared" si="0"/>
+        <v>201</v>
       </c>
       <c r="Y30" s="15" t="str">
         <f>VLOOKUP(X30,MP3_Tab0[[Op]:[Job]],2,0)</f>
-        <v>B</v>
+        <v>F</v>
       </c>
       <c r="Z30" s="15" cm="1">
         <f t="array" aca="1" ref="Z30" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B30),C30,4)</f>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="AA30" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="AB30" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="AC30" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>-14</v>
-      </c>
-      <c r="AC30" s="15">
-        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="AD30" s="15"/>
@@ -18132,62 +18145,62 @@
       </c>
       <c r="AF30" s="9">
         <f ca="1">AVERAGE(MP3_Tab2[C])</f>
-        <v>10.5</v>
+        <v>23.666666666666668</v>
       </c>
       <c r="AG30" s="15"/>
       <c r="AH30" s="37" t="str">
-        <f t="shared" ref="AH30:AH38" si="9">IF(J30="","",J30)</f>
-        <v>B</v>
+        <f t="shared" ref="AH30:AH38" si="8">IF(J30="","",J30)</f>
+        <v>D</v>
       </c>
       <c r="AI30" s="37">
-        <f t="shared" ref="AI30:AI38" si="10">IF(K30="","",K30-L29)</f>
+        <f t="shared" ref="AI30:AI38" si="9">IF(K30="","",K30-L29)</f>
         <v>0</v>
       </c>
       <c r="AJ30" s="37">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="AL30" s="37" t="str">
         <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AL30" s="37" t="str">
-        <f t="shared" si="6"/>
-        <v>E</v>
+        <v>C</v>
       </c>
       <c r="AM30" s="37">
         <f>IF(P30="","",P30-Q29)</f>
         <v>0</v>
       </c>
       <c r="AN30" s="37">
-        <f t="shared" ref="AN30:AN38" si="11">IF(Q30="","",Q30-P30)</f>
-        <v>15</v>
+        <f t="shared" ref="AN30:AN38" si="10">IF(Q30="","",Q30-P30)</f>
+        <v>8</v>
       </c>
       <c r="AP30" s="37" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AQ30" s="37" t="str">
+        <f>IF(U30="","",U30-V29)</f>
+        <v/>
+      </c>
+      <c r="AR30" s="37" t="str">
         <f t="shared" si="7"/>
-        <v>G</v>
-      </c>
-      <c r="AQ30" s="37">
-        <f>IF(U30="","",U30-V29)</f>
-        <v>0</v>
-      </c>
-      <c r="AR30" s="37">
-        <f t="shared" si="8"/>
-        <v>5</v>
+        <v/>
       </c>
     </row>
-    <row r="31" spans="2:50">
+    <row r="31" spans="2:50" x14ac:dyDescent="0.35">
       <c r="B31" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31" s="15">
-        <f t="shared" si="0"/>
-        <v>103</v>
+        <f>B31*100+C31</f>
+        <v>202</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>3</v>
       </c>
       <c r="F31" s="15">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G31" s="15">
         <v>20</v>
@@ -18198,15 +18211,15 @@
       </c>
       <c r="J31" s="15" t="str">
         <f>IF(ISERROR(VLOOKUP(I31,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(I31,MP3_Tab0[[Op]:[Job]],2,0))</f>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="K31" s="15">
-        <f t="shared" ref="K31:K38" si="12">IF(J31="","",IF(ISNUMBER(L30),L30,0))</f>
-        <v>6</v>
+        <f t="shared" ref="K31:K38" si="11">IF(J31="","",IF(ISNUMBER(L30),L30,0))</f>
+        <v>27</v>
       </c>
       <c r="L31" s="15">
         <f>IF(J31="","",K31+VLOOKUP(I31,MP3_Tab0[[Op]:[p]],3,0))</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="M31" s="15"/>
       <c r="N31" s="15">
@@ -18214,15 +18227,15 @@
       </c>
       <c r="O31" s="15" t="str">
         <f>IF(ISERROR(VLOOKUP(N31,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(N31,MP3_Tab0[[Op]:[Job]],2,0))</f>
-        <v/>
-      </c>
-      <c r="P31" s="15" t="str">
-        <f t="shared" ref="P31:P38" si="13">IF(O31="","",IF(ISNUMBER(Q30),Q30,0))</f>
-        <v/>
-      </c>
-      <c r="Q31" s="15" t="str">
+        <v>B</v>
+      </c>
+      <c r="P31" s="15">
+        <f t="shared" ref="P31:P38" si="12">IF(O31="","",IF(ISNUMBER(Q30),Q30,0))</f>
+        <v>23</v>
+      </c>
+      <c r="Q31" s="15">
         <f>IF(O31="","",P31+VLOOKUP(N31,MP3_Tab0[[Op]:[p]],3,0))</f>
-        <v/>
+        <v>30</v>
       </c>
       <c r="R31" s="15"/>
       <c r="S31" s="15">
@@ -18230,20 +18243,20 @@
       </c>
       <c r="T31" s="15" t="str">
         <f>IF(ISERROR(VLOOKUP(S31,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(S31,MP3_Tab0[[Op]:[Job]],2,0))</f>
-        <v>H</v>
-      </c>
-      <c r="U31" s="15">
-        <f t="shared" ref="U31:U38" si="14">IF(T31="","",IF(ISNUMBER(V30),V30,0))</f>
-        <v>6</v>
-      </c>
-      <c r="V31" s="15">
+        <v/>
+      </c>
+      <c r="U31" s="15" t="str">
+        <f t="shared" ref="U31:U38" si="13">IF(T31="","",IF(ISNUMBER(V30),V30,0))</f>
+        <v/>
+      </c>
+      <c r="V31" s="15" t="str">
         <f>IF(T31="","",U31+VLOOKUP(S31,MP3_Tab0[[Op]:[p]],3,0))</f>
-        <v>7</v>
+        <v/>
       </c>
       <c r="W31" s="15"/>
       <c r="X31" s="15">
-        <f t="shared" si="1"/>
-        <v>103</v>
+        <f t="shared" si="0"/>
+        <v>202</v>
       </c>
       <c r="Y31" s="15" t="str">
         <f>VLOOKUP(X31,MP3_Tab0[[Op]:[Job]],2,0)</f>
@@ -18251,19 +18264,19 @@
       </c>
       <c r="Z31" s="15" cm="1">
         <f t="array" aca="1" ref="Z31" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B31),C31,4)</f>
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AA31" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="AB31" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="AC31" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>-5</v>
-      </c>
-      <c r="AC31" s="15">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD31" s="15"/>
       <c r="AE31" t="s">
@@ -18271,62 +18284,62 @@
       </c>
       <c r="AF31" s="9">
         <f ca="1">SUM(MP3_Tab2[T])</f>
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="AG31" s="15"/>
       <c r="AH31" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v>A</v>
+      </c>
+      <c r="AI31" s="37">
         <f t="shared" si="9"/>
-        <v>C</v>
-      </c>
-      <c r="AI31" s="37">
+        <v>0</v>
+      </c>
+      <c r="AJ31" s="37">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AL31" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v>B</v>
+      </c>
+      <c r="AM31" s="37">
+        <f t="shared" ref="AM31:AM38" si="14">IF(P31="","",P31-Q30)</f>
+        <v>0</v>
+      </c>
+      <c r="AN31" s="37">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AJ31" s="37">
-        <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="AL31" s="37" t="str">
+        <v>7</v>
+      </c>
+      <c r="AP31" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AM31" s="37" t="str">
-        <f t="shared" ref="AM31:AM38" si="15">IF(P31="","",P31-Q30)</f>
-        <v/>
-      </c>
-      <c r="AN31" s="37" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="AP31" s="37" t="str">
+      <c r="AQ31" s="37" t="str">
+        <f t="shared" ref="AQ31:AQ38" si="15">IF(U31="","",U31-V30)</f>
+        <v/>
+      </c>
+      <c r="AR31" s="37" t="str">
         <f t="shared" si="7"/>
-        <v>H</v>
-      </c>
-      <c r="AQ31" s="37">
-        <f t="shared" ref="AQ31:AQ38" si="16">IF(U31="","",U31-V30)</f>
-        <v>0</v>
-      </c>
-      <c r="AR31" s="37">
-        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:50" x14ac:dyDescent="0.35">
+      <c r="B32" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:50">
-      <c r="B32" s="13">
+      <c r="C32" s="13">
         <v>2</v>
       </c>
-      <c r="C32" s="13">
-        <v>1</v>
-      </c>
       <c r="D32" s="15">
-        <f t="shared" si="0"/>
-        <v>201</v>
+        <f>B32*100+C32</f>
+        <v>102</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>6</v>
       </c>
       <c r="F32" s="15">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G32" s="15">
         <v>20</v>
@@ -18340,7 +18353,7 @@
         <v/>
       </c>
       <c r="K32" s="15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L32" s="15" t="str">
@@ -18356,7 +18369,7 @@
         <v/>
       </c>
       <c r="P32" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="Q32" s="15" t="str">
@@ -18369,20 +18382,20 @@
       </c>
       <c r="T32" s="15" t="str">
         <f>IF(ISERROR(VLOOKUP(S32,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(S32,MP3_Tab0[[Op]:[Job]],2,0))</f>
-        <v>I</v>
-      </c>
-      <c r="U32" s="15">
-        <f t="shared" si="14"/>
-        <v>7</v>
-      </c>
-      <c r="V32" s="15">
+        <v/>
+      </c>
+      <c r="U32" s="15" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="V32" s="15" t="str">
         <f>IF(T32="","",U32+VLOOKUP(S32,MP3_Tab0[[Op]:[p]],3,0))</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="W32" s="15"/>
       <c r="X32" s="15">
-        <f t="shared" si="1"/>
-        <v>201</v>
+        <f t="shared" si="0"/>
+        <v>102</v>
       </c>
       <c r="Y32" s="15" t="str">
         <f>VLOOKUP(X32,MP3_Tab0[[Op]:[Job]],2,0)</f>
@@ -18390,19 +18403,19 @@
       </c>
       <c r="Z32" s="15" cm="1">
         <f t="array" aca="1" ref="Z32" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B32),C32,4)</f>
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="AA32" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="AB32" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="AC32" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>-8</v>
-      </c>
-      <c r="AC32" s="15">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AD32" s="15"/>
       <c r="AE32" t="s">
@@ -18410,62 +18423,62 @@
       </c>
       <c r="AF32" s="9">
         <f ca="1">MAX(MP3_Tab2[T])</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="AG32" s="15"/>
       <c r="AH32" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AI32" s="37" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AI32" s="37" t="str">
+      <c r="AJ32" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AL32" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AM32" s="37" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="AN32" s="37" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AJ32" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AL32" s="37" t="str">
+      <c r="AP32" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AM32" s="37" t="str">
+      <c r="AQ32" s="37" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AN32" s="37" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="AP32" s="37" t="str">
+      <c r="AR32" s="37" t="str">
         <f t="shared" si="7"/>
-        <v>I</v>
-      </c>
-      <c r="AQ32" s="37">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AR32" s="37">
-        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="B33" s="13">
+        <v>1</v>
+      </c>
+      <c r="C33" s="13">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:44">
-      <c r="B33" s="15">
-        <v>2</v>
-      </c>
-      <c r="C33" s="13">
-        <v>2</v>
-      </c>
       <c r="D33" s="15">
-        <f t="shared" si="0"/>
-        <v>202</v>
+        <f>B33*100+C33</f>
+        <v>103</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F33" s="15">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G33" s="15">
         <v>20</v>
@@ -18479,7 +18492,7 @@
         <v/>
       </c>
       <c r="K33" s="15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L33" s="15" t="str">
@@ -18495,7 +18508,7 @@
         <v/>
       </c>
       <c r="P33" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="Q33" s="15" t="str">
@@ -18508,40 +18521,40 @@
       </c>
       <c r="T33" s="15" t="str">
         <f>IF(ISERROR(VLOOKUP(S33,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(S33,MP3_Tab0[[Op]:[Job]],2,0))</f>
-        <v>J</v>
-      </c>
-      <c r="U33" s="15">
-        <f t="shared" si="14"/>
-        <v>10</v>
-      </c>
-      <c r="V33" s="15">
+        <v/>
+      </c>
+      <c r="U33" s="15" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="V33" s="15" t="str">
         <f>IF(T33="","",U33+VLOOKUP(S33,MP3_Tab0[[Op]:[p]],3,0))</f>
-        <v>17</v>
+        <v/>
       </c>
       <c r="W33" s="15"/>
       <c r="X33" s="15">
-        <f t="shared" si="1"/>
-        <v>202</v>
+        <f t="shared" si="0"/>
+        <v>103</v>
       </c>
       <c r="Y33" s="15" t="str">
         <f>VLOOKUP(X33,MP3_Tab0[[Op]:[Job]],2,0)</f>
-        <v>E</v>
+        <v>A</v>
       </c>
       <c r="Z33" s="15" cm="1">
         <f t="array" aca="1" ref="Z33" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B33),C33,4)</f>
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="AA33" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="AB33" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="AC33" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="AC33" s="15">
-        <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="AD33" s="15"/>
       <c r="AE33" t="s">
@@ -18549,64 +18562,64 @@
       </c>
       <c r="AF33" s="25">
         <f ca="1">COUNTIF(MP3_Tab2[T],"&gt;0")</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AG33" s="15"/>
       <c r="AH33" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AI33" s="37" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AI33" s="37" t="str">
+      <c r="AJ33" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AL33" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AM33" s="37" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="AN33" s="37" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AJ33" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AL33" s="37" t="str">
+      <c r="AP33" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AM33" s="37" t="str">
+      <c r="AQ33" s="37" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AN33" s="37" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="AP33" s="37" t="str">
+      <c r="AR33" s="37" t="str">
         <f t="shared" si="7"/>
-        <v>J</v>
-      </c>
-      <c r="AQ33" s="37">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AR33" s="37">
-        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="B34" s="13">
+        <v>2</v>
+      </c>
+      <c r="C34" s="13">
+        <v>3</v>
+      </c>
+      <c r="D34" s="15">
+        <f>B34*100+C34</f>
+        <v>203</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="15">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:44">
-      <c r="B34" s="15">
-        <v>3</v>
-      </c>
-      <c r="C34" s="13">
-        <v>1</v>
-      </c>
-      <c r="D34" s="15">
-        <f t="shared" si="0"/>
-        <v>301</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="15">
-        <v>1</v>
-      </c>
-      <c r="G34" s="13">
+      <c r="G34" s="15">
         <v>20</v>
       </c>
       <c r="I34" s="15">
@@ -18617,7 +18630,7 @@
         <v/>
       </c>
       <c r="K34" s="15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L34" s="15" t="str">
@@ -18632,7 +18645,7 @@
         <v/>
       </c>
       <c r="P34" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="Q34" s="15" t="str">
@@ -18647,7 +18660,7 @@
         <v/>
       </c>
       <c r="U34" s="15" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="V34" s="15" t="str">
@@ -18655,234 +18668,203 @@
         <v/>
       </c>
       <c r="X34" s="15">
-        <f t="shared" si="1"/>
-        <v>301</v>
+        <f t="shared" si="0"/>
+        <v>203</v>
       </c>
       <c r="Y34" s="15" t="str">
         <f>VLOOKUP(X34,MP3_Tab0[[Op]:[Job]],2,0)</f>
-        <v>F</v>
+        <v>B</v>
       </c>
       <c r="Z34" s="15" cm="1">
         <f t="array" aca="1" ref="Z34" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B34),C34,4)</f>
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="AA34" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="AB34" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="AC34" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>-19</v>
-      </c>
-      <c r="AC34" s="15">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD34" s="15"/>
       <c r="AE34" s="15"/>
       <c r="AF34" s="15"/>
       <c r="AG34" s="15"/>
       <c r="AH34" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AI34" s="37" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AI34" s="37" t="str">
+      <c r="AJ34" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AL34" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AM34" s="37" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="AN34" s="37" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AJ34" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AL34" s="37" t="str">
+      <c r="AP34" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AM34" s="37" t="str">
+      <c r="AQ34" s="37" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AN34" s="37" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="AP34" s="37" t="str">
+      <c r="AR34" s="37" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="AQ34" s="37" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="AR34" s="37" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
     </row>
-    <row r="35" spans="1:44">
-      <c r="B35" s="15">
-        <v>3</v>
-      </c>
-      <c r="C35" s="13">
-        <v>2</v>
-      </c>
-      <c r="D35" s="15">
-        <f t="shared" si="0"/>
-        <v>302</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="15">
-        <v>5</v>
-      </c>
-      <c r="G35" s="13">
-        <v>20</v>
-      </c>
+    <row r="35" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="B35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
       <c r="I35" s="15">
         <v>107</v>
       </c>
-      <c r="J35" s="15" t="str">
+      <c r="J35" s="50" t="str">
         <f>IF(ISERROR(VLOOKUP(I35,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(I35,MP3_Tab0[[Op]:[Job]],2,0))</f>
         <v/>
       </c>
       <c r="K35" s="15" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="L35" s="15" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="L35" s="50" t="str">
         <f>IF(J35="","",K35+VLOOKUP(I35,MP3_Tab0[[Op]:[p]],3,0))</f>
         <v/>
       </c>
       <c r="N35" s="15">
         <v>207</v>
       </c>
-      <c r="O35" s="15" t="str">
+      <c r="O35" s="50" t="str">
         <f>IF(ISERROR(VLOOKUP(N35,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(N35,MP3_Tab0[[Op]:[Job]],2,0))</f>
         <v/>
       </c>
       <c r="P35" s="15" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="Q35" s="15" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="Q35" s="50" t="str">
         <f>IF(O35="","",P35+VLOOKUP(N35,MP3_Tab0[[Op]:[p]],3,0))</f>
         <v/>
       </c>
       <c r="S35" s="15">
         <v>307</v>
       </c>
-      <c r="T35" s="15" t="str">
+      <c r="T35" s="50" t="str">
         <f>IF(ISERROR(VLOOKUP(S35,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(S35,MP3_Tab0[[Op]:[Job]],2,0))</f>
         <v/>
       </c>
       <c r="U35" s="15" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="V35" s="15" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="V35" s="50" t="str">
         <f>IF(T35="","",U35+VLOOKUP(S35,MP3_Tab0[[Op]:[p]],3,0))</f>
         <v/>
       </c>
-      <c r="X35" s="15">
+      <c r="X35" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y35" s="50" t="e">
+        <f>VLOOKUP(X35,MP3_Tab0[[Op]:[Job]],2,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z35" s="50" t="e" cm="1">
+        <f t="array" aca="1" ref="Z35" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B35),C35,4)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AA35" s="50">
         <f t="shared" si="1"/>
-        <v>302</v>
-      </c>
-      <c r="Y35" s="15" t="str">
-        <f>VLOOKUP(X35,MP3_Tab0[[Op]:[Job]],2,0)</f>
-        <v>G</v>
-      </c>
-      <c r="Z35" s="15" cm="1">
-        <f t="array" aca="1" ref="Z35" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B35),C35,4)</f>
-        <v>6</v>
-      </c>
-      <c r="AA35" s="15">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="AB35" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="50" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AC35" s="50" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>-14</v>
-      </c>
-      <c r="AC35" s="15">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="AD35" s="15"/>
       <c r="AE35" s="15"/>
       <c r="AF35" s="15"/>
       <c r="AG35" s="15"/>
       <c r="AH35" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AI35" s="37" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AI35" s="37" t="str">
+      <c r="AJ35" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AL35" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AM35" s="37" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="AN35" s="37" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AJ35" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AL35" s="37" t="str">
+      <c r="AP35" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AM35" s="37" t="str">
+      <c r="AQ35" s="37" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AN35" s="37" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="AP35" s="37" t="str">
+      <c r="AR35" s="37" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="AQ35" s="37" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="AR35" s="37" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
     </row>
-    <row r="36" spans="1:44">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A36" s="15"/>
-      <c r="B36" s="13">
-        <v>3</v>
-      </c>
-      <c r="C36" s="13">
-        <v>3</v>
-      </c>
-      <c r="D36" s="15">
-        <f t="shared" si="0"/>
-        <v>303</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F36" s="15">
-        <v>1</v>
-      </c>
-      <c r="G36" s="13">
-        <v>20</v>
-      </c>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
       <c r="H36" s="15"/>
       <c r="I36" s="15">
         <v>108</v>
       </c>
-      <c r="J36" s="15" t="str">
+      <c r="J36" s="50" t="str">
         <f>IF(ISERROR(VLOOKUP(I36,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(I36,MP3_Tab0[[Op]:[Job]],2,0))</f>
         <v/>
       </c>
       <c r="K36" s="15" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="L36" s="15" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="L36" s="50" t="str">
         <f>IF(J36="","",K36+VLOOKUP(I36,MP3_Tab0[[Op]:[p]],3,0))</f>
         <v/>
       </c>
@@ -18890,132 +18872,116 @@
       <c r="N36" s="15">
         <v>208</v>
       </c>
-      <c r="O36" s="15" t="str">
+      <c r="O36" s="50" t="str">
         <f>IF(ISERROR(VLOOKUP(N36,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(N36,MP3_Tab0[[Op]:[Job]],2,0))</f>
         <v/>
       </c>
       <c r="P36" s="15" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="Q36" s="15" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="Q36" s="50" t="str">
         <f>IF(O36="","",P36+VLOOKUP(N36,MP3_Tab0[[Op]:[p]],3,0))</f>
         <v/>
       </c>
       <c r="S36" s="15">
         <v>308</v>
       </c>
-      <c r="T36" s="15" t="str">
+      <c r="T36" s="50" t="str">
         <f>IF(ISERROR(VLOOKUP(S36,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(S36,MP3_Tab0[[Op]:[Job]],2,0))</f>
         <v/>
       </c>
       <c r="U36" s="15" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="V36" s="15" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="V36" s="50" t="str">
         <f>IF(T36="","",U36+VLOOKUP(S36,MP3_Tab0[[Op]:[p]],3,0))</f>
         <v/>
       </c>
       <c r="X36" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y36" s="15" t="e">
+        <f>VLOOKUP(X36,MP3_Tab0[[Op]:[Job]],2,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z36" s="15" t="e" cm="1">
+        <f t="array" aca="1" ref="Z36" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B36),C36,4)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AA36" s="15">
         <f t="shared" si="1"/>
-        <v>303</v>
-      </c>
-      <c r="Y36" s="15" t="str">
-        <f>VLOOKUP(X36,MP3_Tab0[[Op]:[Job]],2,0)</f>
-        <v>H</v>
-      </c>
-      <c r="Z36" s="15" cm="1">
-        <f t="array" aca="1" ref="Z36" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B36),C36,4)</f>
-        <v>7</v>
-      </c>
-      <c r="AA36" s="15">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="AB36" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="15" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AC36" s="15" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>-13</v>
-      </c>
-      <c r="AC36" s="15">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="AD36" s="15"/>
       <c r="AE36" s="15"/>
       <c r="AF36" s="15"/>
       <c r="AG36" s="15"/>
       <c r="AH36" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AI36" s="37" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AI36" s="37" t="str">
+      <c r="AJ36" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AL36" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AM36" s="37" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="AN36" s="37" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AJ36" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AL36" s="37" t="str">
+      <c r="AP36" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AM36" s="37" t="str">
+      <c r="AQ36" s="37" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AN36" s="37" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="AP36" s="37" t="str">
+      <c r="AR36" s="37" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="AQ36" s="37" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="AR36" s="37" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
     </row>
-    <row r="37" spans="1:44">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A37" s="15"/>
-      <c r="B37" s="13">
-        <v>3</v>
-      </c>
-      <c r="C37" s="13">
-        <v>4</v>
-      </c>
-      <c r="D37" s="15">
-        <f t="shared" si="0"/>
-        <v>304</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37" s="15">
-        <v>3</v>
-      </c>
-      <c r="G37" s="13">
-        <v>20</v>
-      </c>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
       <c r="H37" s="15"/>
       <c r="I37" s="15">
         <v>109</v>
       </c>
-      <c r="J37" s="15" t="str">
+      <c r="J37" s="50" t="str">
         <f>IF(ISERROR(VLOOKUP(I37,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(I37,MP3_Tab0[[Op]:[Job]],2,0))</f>
         <v/>
       </c>
       <c r="K37" s="15" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="L37" s="15" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="L37" s="50" t="str">
         <f>IF(J37="","",K37+VLOOKUP(I37,MP3_Tab0[[Op]:[p]],3,0))</f>
         <v/>
       </c>
@@ -19028,7 +18994,7 @@
         <v/>
       </c>
       <c r="P37" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="Q37" s="15" t="str">
@@ -19043,7 +19009,7 @@
         <v/>
       </c>
       <c r="U37" s="15" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="V37" s="15" t="str">
@@ -19051,104 +19017,86 @@
         <v/>
       </c>
       <c r="X37" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y37" s="15" t="e">
+        <f>VLOOKUP(X37,MP3_Tab0[[Op]:[Job]],2,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z37" s="15" t="e" cm="1">
+        <f t="array" aca="1" ref="Z37" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B37),C37,4)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AA37" s="15">
         <f t="shared" si="1"/>
-        <v>304</v>
-      </c>
-      <c r="Y37" s="15" t="str">
-        <f>VLOOKUP(X37,MP3_Tab0[[Op]:[Job]],2,0)</f>
-        <v>I</v>
-      </c>
-      <c r="Z37" s="15" cm="1">
-        <f t="array" aca="1" ref="Z37" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B37),C37,4)</f>
-        <v>10</v>
-      </c>
-      <c r="AA37" s="15">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="AB37" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="15" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AC37" s="15" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>-10</v>
-      </c>
-      <c r="AC37" s="15">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="AD37" s="15"/>
       <c r="AE37" s="15"/>
       <c r="AF37" s="15"/>
       <c r="AG37" s="15"/>
       <c r="AH37" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AI37" s="37" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AI37" s="37" t="str">
+      <c r="AJ37" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AL37" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AM37" s="37" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="AN37" s="37" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AJ37" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AL37" s="37" t="str">
+      <c r="AP37" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AM37" s="37" t="str">
+      <c r="AQ37" s="37" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AN37" s="37" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="AP37" s="37" t="str">
+      <c r="AR37" s="37" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="AQ37" s="37" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="AR37" s="37" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
     </row>
-    <row r="38" spans="1:44">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A38" s="15"/>
-      <c r="B38" s="13">
-        <v>3</v>
-      </c>
-      <c r="C38" s="13">
-        <v>5</v>
-      </c>
-      <c r="D38" s="15">
-        <f t="shared" si="0"/>
-        <v>305</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F38" s="13">
-        <v>7</v>
-      </c>
-      <c r="G38" s="13">
-        <v>20</v>
-      </c>
+      <c r="D38" s="15"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15">
         <v>110</v>
       </c>
-      <c r="J38" s="15" t="str">
+      <c r="J38" s="50" t="str">
         <f>IF(ISERROR(VLOOKUP(I38,MP3_Tab0[[Op]:[Job]],2,0)),"",VLOOKUP(I38,MP3_Tab0[[Op]:[Job]],2,0))</f>
         <v/>
       </c>
       <c r="K38" s="15" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="L38" s="15" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="L38" s="50" t="str">
         <f>IF(J38="","",K38+VLOOKUP(I38,MP3_Tab0[[Op]:[p]],3,0))</f>
         <v/>
       </c>
@@ -19161,7 +19109,7 @@
         <v/>
       </c>
       <c r="P38" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="Q38" s="15" t="str">
@@ -19176,7 +19124,7 @@
         <v/>
       </c>
       <c r="U38" s="15" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="V38" s="15" t="str">
@@ -19184,71 +19132,71 @@
         <v/>
       </c>
       <c r="X38" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y38" s="15" t="e">
+        <f>VLOOKUP(X38,MP3_Tab0[[Op]:[Job]],2,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z38" s="15" t="e" cm="1">
+        <f t="array" aca="1" ref="Z38" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B38),C38,4)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AA38" s="15">
         <f t="shared" si="1"/>
-        <v>305</v>
-      </c>
-      <c r="Y38" s="15" t="str">
-        <f>VLOOKUP(X38,MP3_Tab0[[Op]:[Job]],2,0)</f>
-        <v>J</v>
-      </c>
-      <c r="Z38" s="15" cm="1">
-        <f t="array" aca="1" ref="Z38" ca="1">INDEX(INDIRECT("MP3_TabM"&amp;B38),C38,4)</f>
-        <v>17</v>
-      </c>
-      <c r="AA38" s="15">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="AB38" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="15" t="e">
+        <f t="shared" ca="1" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AC38" s="15" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>-3</v>
-      </c>
-      <c r="AC38" s="15">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="AD38" s="15"/>
       <c r="AE38" s="15"/>
       <c r="AF38" s="15"/>
       <c r="AG38" s="15"/>
       <c r="AH38" s="37" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AI38" s="37" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AI38" s="37" t="str">
+      <c r="AJ38" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AL38" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AM38" s="37" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="AN38" s="37" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AJ38" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AL38" s="37" t="str">
+      <c r="AP38" s="37" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AM38" s="37" t="str">
+      <c r="AQ38" s="37" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AN38" s="37" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="AP38" s="37" t="str">
+      <c r="AR38" s="37" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="AQ38" s="37" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="AR38" s="37" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
     </row>
-    <row r="39" spans="1:44">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A39" s="15"/>
       <c r="B39" s="33"/>
       <c r="C39" s="33"/>
@@ -19267,7 +19215,7 @@
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
     </row>
-    <row r="40" spans="1:44">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -19285,7 +19233,7 @@
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
     </row>
-    <row r="41" spans="1:44">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -19303,7 +19251,7 @@
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
     </row>
-    <row r="42" spans="1:44">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -19321,7 +19269,7 @@
       <c r="Q42" s="15"/>
       <c r="R42" s="15"/>
     </row>
-    <row r="43" spans="1:44">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -19339,7 +19287,7 @@
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
     </row>
-    <row r="44" spans="1:44">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -19357,21 +19305,21 @@
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
     </row>
-    <row r="45" spans="1:44">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
     </row>
-    <row r="46" spans="1:44">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
     </row>
-    <row r="47" spans="1:44">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
       <c r="F47" s="15"/>
@@ -19419,7 +19367,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="21" width="5.6328125" style="13" customWidth="1"/>
     <col min="22" max="22" width="20.6328125" style="13" customWidth="1"/>
@@ -19427,9 +19375,9 @@
     <col min="32" max="16384" width="8.90625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="12" customFormat="1" ht="26">
+    <row r="1" spans="1:33" s="12" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="10"/>
@@ -19455,7 +19403,7 @@
       <c r="W1" s="10"/>
       <c r="X1" s="10"/>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -19469,7 +19417,7 @@
       <c r="AC3"/>
       <c r="AD3"/>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -19486,7 +19434,7 @@
       <c r="AF4" s="15"/>
       <c r="AG4" s="15"/>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -19501,7 +19449,7 @@
       <c r="AD5"/>
       <c r="AE5" s="15"/>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -19516,7 +19464,7 @@
       <c r="AD6"/>
       <c r="AE6" s="15"/>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -19530,7 +19478,7 @@
       <c r="AC7"/>
       <c r="AD7"/>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -19544,7 +19492,7 @@
       <c r="AC8"/>
       <c r="AD8"/>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -19558,7 +19506,7 @@
       <c r="AC9"/>
       <c r="AD9"/>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -19572,7 +19520,7 @@
       <c r="AC10"/>
       <c r="AD10"/>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -19588,7 +19536,7 @@
       <c r="AD11"/>
       <c r="AE11" s="15"/>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -19604,7 +19552,7 @@
       <c r="AD12"/>
       <c r="AE12" s="15"/>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -19620,36 +19568,36 @@
       <c r="AD13" s="15"/>
       <c r="AE13" s="15"/>
     </row>
-    <row r="18" spans="2:31">
+    <row r="18" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B18" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="47" t="s">
+      <c r="H18" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="L18" s="47" t="s">
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="L18" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
       <c r="U18" s="15"/>
       <c r="V18" s="15"/>
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
-      <c r="Y18" s="46" t="s">
+      <c r="Y18" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="Z18" s="46"/>
-      <c r="AA18" s="46"/>
-      <c r="AC18" s="46" t="s">
+      <c r="Z18" s="45"/>
+      <c r="AA18" s="45"/>
+      <c r="AC18" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="AD18" s="46"/>
-      <c r="AE18" s="46"/>
+      <c r="AD18" s="45"/>
+      <c r="AE18" s="45"/>
     </row>
-    <row r="19" spans="2:31">
+    <row r="19" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B19" s="15"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -19674,7 +19622,7 @@
       <c r="AD19" s="15"/>
       <c r="AE19" s="15"/>
     </row>
-    <row r="20" spans="2:31" customFormat="1" ht="13">
+    <row r="20" spans="2:31" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="B20" s="41" t="s">
         <v>0</v>
       </c>
@@ -19682,10 +19630,10 @@
         <v>1</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F20" s="41" t="s">
         <v>10</v>
@@ -19724,7 +19672,7 @@
         <v>11</v>
       </c>
       <c r="V20" s="41" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="W20" s="41" t="s">
         <v>25</v>
@@ -19736,7 +19684,7 @@
         <v>14</v>
       </c>
       <c r="AA20" s="41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AC20" s="41" t="s">
         <v>1</v>
@@ -19745,10 +19693,10 @@
         <v>14</v>
       </c>
       <c r="AE20" s="41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="21" spans="2:31">
+    <row r="21" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B21" s="15"/>
       <c r="C21" s="15" t="s">
         <v>4</v>
@@ -19841,7 +19789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:31">
+    <row r="22" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B22" s="15"/>
       <c r="C22" s="15" t="s">
         <v>5</v>
@@ -19934,7 +19882,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:31">
+    <row r="23" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B23" s="15"/>
       <c r="C23" s="15" t="s">
         <v>3</v>
@@ -20027,7 +19975,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:31">
+    <row r="24" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B24" s="15"/>
       <c r="C24" s="15" t="s">
         <v>6</v>
@@ -20120,7 +20068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:31">
+    <row r="25" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B25" s="15"/>
       <c r="C25" s="15" t="s">
         <v>7</v>
@@ -20213,7 +20161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:31">
+    <row r="26" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -20245,7 +20193,7 @@
       <c r="AD26" s="15"/>
       <c r="AE26" s="15"/>
     </row>
-    <row r="27" spans="2:31">
+    <row r="27" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -20273,7 +20221,7 @@
       <c r="AD27" s="17"/>
       <c r="AE27" s="17"/>
     </row>
-    <row r="28" spans="2:31">
+    <row r="28" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B28" s="24"/>
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
@@ -20294,7 +20242,7 @@
       <c r="S28" s="14"/>
       <c r="T28" s="14"/>
     </row>
-    <row r="29" spans="2:31">
+    <row r="29" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
@@ -20349,7 +20297,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.6328125" customWidth="1"/>
     <col min="2" max="41" width="5.6328125" style="1" customWidth="1"/>
@@ -20358,7 +20306,7 @@
     <col min="65" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="26">
+    <row r="1" spans="1:58" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -20392,7 +20340,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:58">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.35">
       <c r="AI2"/>
       <c r="AJ2"/>
       <c r="AK2"/>
@@ -20412,7 +20360,7 @@
       <c r="BE2"/>
       <c r="BF2"/>
     </row>
-    <row r="3" spans="1:58">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.35">
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
@@ -20434,12 +20382,12 @@
       <c r="T3" s="40"/>
       <c r="U3" s="40"/>
     </row>
-    <row r="4" spans="1:58">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.35">
       <c r="X4" s="42" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="AC4" s="32" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="AN4"/>
       <c r="AR4"/>
@@ -20455,7 +20403,7 @@
       <c r="BE4"/>
       <c r="BF4"/>
     </row>
-    <row r="5" spans="1:58">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
       <c r="X5" s="42" t="s">
         <v>4</v>
       </c>
@@ -20494,7 +20442,7 @@
       <c r="BE5"/>
       <c r="BF5"/>
     </row>
-    <row r="6" spans="1:58">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.35">
       <c r="X6" s="42" t="s">
         <v>5</v>
       </c>
@@ -20533,7 +20481,7 @@
       <c r="BE6"/>
       <c r="BF6"/>
     </row>
-    <row r="7" spans="1:58">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.35">
       <c r="X7" s="42" t="s">
         <v>3</v>
       </c>
@@ -20572,7 +20520,7 @@
       <c r="BE7"/>
       <c r="BF7"/>
     </row>
-    <row r="8" spans="1:58">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.35">
       <c r="X8" s="42" t="s">
         <v>6</v>
       </c>
@@ -20596,7 +20544,7 @@
       <c r="BE8"/>
       <c r="BF8"/>
     </row>
-    <row r="9" spans="1:58">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.35">
       <c r="X9" s="42" t="s">
         <v>7</v>
       </c>
@@ -20620,7 +20568,7 @@
       <c r="BE9"/>
       <c r="BF9"/>
     </row>
-    <row r="10" spans="1:58">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.35">
       <c r="AN10"/>
       <c r="AR10"/>
       <c r="AS10"/>
@@ -20635,9 +20583,9 @@
       <c r="BE10"/>
       <c r="BF10"/>
     </row>
-    <row r="11" spans="1:58">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.35">
       <c r="AC11" s="32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="AN11"/>
       <c r="AR11"/>
@@ -20653,7 +20601,7 @@
       <c r="BE11"/>
       <c r="BF11"/>
     </row>
-    <row r="12" spans="1:58">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.35">
       <c r="AD12" s="43" t="s">
         <v>27</v>
       </c>
@@ -20683,7 +20631,7 @@
       <c r="BE12"/>
       <c r="BF12"/>
     </row>
-    <row r="13" spans="1:58">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.35">
       <c r="AD13" s="43" t="s">
         <v>30</v>
       </c>
@@ -20710,7 +20658,7 @@
       <c r="BE13"/>
       <c r="BF13"/>
     </row>
-    <row r="14" spans="1:58">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.35">
       <c r="AD14" s="43" t="s">
         <v>31</v>
       </c>
@@ -20740,7 +20688,7 @@
       <c r="BE14"/>
       <c r="BF14"/>
     </row>
-    <row r="15" spans="1:58">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.35">
       <c r="AN15"/>
       <c r="AR15"/>
       <c r="AS15"/>
@@ -20755,7 +20703,7 @@
       <c r="BE15"/>
       <c r="BF15"/>
     </row>
-    <row r="16" spans="1:58">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.35">
       <c r="AN16"/>
       <c r="AR16"/>
       <c r="AS16"/>
@@ -20770,7 +20718,7 @@
       <c r="BE16"/>
       <c r="BF16"/>
     </row>
-    <row r="17" spans="2:65">
+    <row r="17" spans="2:65" x14ac:dyDescent="0.35">
       <c r="AN17"/>
       <c r="AR17"/>
       <c r="AS17"/>
@@ -20785,9 +20733,9 @@
       <c r="BE17"/>
       <c r="BF17"/>
     </row>
-    <row r="18" spans="2:65">
+    <row r="18" spans="2:65" x14ac:dyDescent="0.35">
       <c r="AC18" s="32" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="AN18"/>
       <c r="AR18"/>
@@ -20803,7 +20751,7 @@
       <c r="BE18"/>
       <c r="BF18"/>
     </row>
-    <row r="19" spans="2:65">
+    <row r="19" spans="2:65" x14ac:dyDescent="0.35">
       <c r="AD19" s="43" t="s">
         <v>27</v>
       </c>
@@ -20833,7 +20781,7 @@
       <c r="BE19"/>
       <c r="BF19"/>
     </row>
-    <row r="20" spans="2:65">
+    <row r="20" spans="2:65" x14ac:dyDescent="0.35">
       <c r="AD20" s="43" t="s">
         <v>30</v>
       </c>
@@ -20860,7 +20808,7 @@
       <c r="BE20"/>
       <c r="BF20"/>
     </row>
-    <row r="21" spans="2:65">
+    <row r="21" spans="2:65" x14ac:dyDescent="0.35">
       <c r="AD21" s="43" t="s">
         <v>31</v>
       </c>
@@ -20890,7 +20838,7 @@
       <c r="BE21"/>
       <c r="BF21"/>
     </row>
-    <row r="22" spans="2:65">
+    <row r="22" spans="2:65" x14ac:dyDescent="0.35">
       <c r="AD22"/>
       <c r="AE22"/>
       <c r="AF22"/>
@@ -20910,7 +20858,7 @@
       <c r="BE22"/>
       <c r="BF22"/>
     </row>
-    <row r="23" spans="2:65">
+    <row r="23" spans="2:65" x14ac:dyDescent="0.35">
       <c r="AI23"/>
       <c r="AJ23"/>
       <c r="AK23"/>
@@ -20930,7 +20878,7 @@
       <c r="BE23"/>
       <c r="BF23"/>
     </row>
-    <row r="24" spans="2:65">
+    <row r="24" spans="2:65" x14ac:dyDescent="0.35">
       <c r="AI24"/>
       <c r="AJ24"/>
       <c r="AK24"/>
@@ -20949,7 +20897,7 @@
       <c r="BD24"/>
       <c r="BE24"/>
     </row>
-    <row r="25" spans="2:65">
+    <row r="25" spans="2:65" x14ac:dyDescent="0.35">
       <c r="V25" s="7"/>
       <c r="AJ25"/>
       <c r="AK25"/>
@@ -20964,22 +20912,22 @@
       <c r="BI25" s="6"/>
       <c r="BJ25" s="38"/>
     </row>
-    <row r="26" spans="2:65">
-      <c r="L26" s="48" t="s">
+    <row r="26" spans="2:65" x14ac:dyDescent="0.35">
+      <c r="L26" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="M26" s="48"/>
-      <c r="N26" s="48"/>
-      <c r="P26" s="48" t="s">
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
+      <c r="P26" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="Q26" s="48"/>
-      <c r="R26" s="48"/>
-      <c r="T26" s="48" t="s">
+      <c r="Q26" s="47"/>
+      <c r="R26" s="47"/>
+      <c r="T26" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="U26" s="48"/>
-      <c r="V26" s="48"/>
+      <c r="U26" s="47"/>
+      <c r="V26" s="47"/>
       <c r="AJ26"/>
       <c r="AK26"/>
       <c r="AL26"/>
@@ -20990,7 +20938,7 @@
       <c r="AT26"/>
       <c r="AY26"/>
     </row>
-    <row r="27" spans="2:65">
+    <row r="27" spans="2:65" x14ac:dyDescent="0.35">
       <c r="L27" s="7" t="s">
         <v>24</v>
       </c>
@@ -21009,32 +20957,32 @@
       <c r="AM27"/>
       <c r="AN27"/>
       <c r="AO27"/>
-      <c r="AS27" s="48" t="s">
+      <c r="AS27" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="AT27" s="48"/>
-      <c r="AU27" s="48"/>
-      <c r="AV27" s="48"/>
-      <c r="AW27" s="48"/>
-      <c r="AX27" s="48"/>
-      <c r="AZ27" s="48" t="s">
+      <c r="AT27" s="47"/>
+      <c r="AU27" s="47"/>
+      <c r="AV27" s="47"/>
+      <c r="AW27" s="47"/>
+      <c r="AX27" s="47"/>
+      <c r="AZ27" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="BA27" s="48"/>
-      <c r="BB27" s="48"/>
-      <c r="BC27" s="48"/>
-      <c r="BD27" s="48"/>
-      <c r="BE27" s="48"/>
-      <c r="BG27" s="48" t="s">
+      <c r="BA27" s="47"/>
+      <c r="BB27" s="47"/>
+      <c r="BC27" s="47"/>
+      <c r="BD27" s="47"/>
+      <c r="BE27" s="47"/>
+      <c r="BG27" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="BH27" s="48"/>
-      <c r="BI27" s="48"/>
-      <c r="BJ27" s="48"/>
-      <c r="BK27" s="48"/>
-      <c r="BL27" s="48"/>
+      <c r="BH27" s="47"/>
+      <c r="BI27" s="47"/>
+      <c r="BJ27" s="47"/>
+      <c r="BK27" s="47"/>
+      <c r="BL27" s="47"/>
     </row>
-    <row r="28" spans="2:65">
+    <row r="28" spans="2:65" x14ac:dyDescent="0.35">
       <c r="L28"/>
       <c r="N28"/>
       <c r="P28"/>
@@ -21062,7 +21010,7 @@
       <c r="BH28"/>
       <c r="BI28"/>
     </row>
-    <row r="29" spans="2:65" customFormat="1" ht="13">
+    <row r="29" spans="2:65" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="B29" s="41" t="s">
         <v>1</v>
       </c>
@@ -21130,10 +21078,10 @@
         <v>2</v>
       </c>
       <c r="AC29" s="41" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AD29" s="41" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AE29" s="41" t="s">
         <v>15</v>
@@ -21163,7 +21111,7 @@
         <v>11</v>
       </c>
       <c r="AP29" s="41" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AQ29" s="41" t="s">
         <v>25</v>
@@ -21184,7 +21132,7 @@
         <v>14</v>
       </c>
       <c r="AX29" s="41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AZ29" s="41" t="s">
         <v>23</v>
@@ -21202,7 +21150,7 @@
         <v>14</v>
       </c>
       <c r="BE29" s="41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="BG29" s="41" t="s">
         <v>23</v>
@@ -21220,10 +21168,10 @@
         <v>14</v>
       </c>
       <c r="BL29" s="41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="30" spans="2:65">
+    <row r="30" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>4</v>
       </c>
@@ -21424,7 +21372,7 @@
       </c>
       <c r="BM30"/>
     </row>
-    <row r="31" spans="2:65">
+    <row r="31" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>5</v>
       </c>
@@ -21625,7 +21573,7 @@
       </c>
       <c r="BM31"/>
     </row>
-    <row r="32" spans="2:65">
+    <row r="32" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>3</v>
       </c>
@@ -21826,7 +21774,7 @@
       </c>
       <c r="BM32"/>
     </row>
-    <row r="33" spans="2:65">
+    <row r="33" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -22021,7 +21969,7 @@
       </c>
       <c r="BM33"/>
     </row>
-    <row r="34" spans="2:65">
+    <row r="34" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>7</v>
       </c>
@@ -22204,7 +22152,7 @@
       </c>
       <c r="BM34"/>
     </row>
-    <row r="35" spans="2:65">
+    <row r="35" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
@@ -22357,7 +22305,7 @@
       </c>
       <c r="BM35"/>
     </row>
-    <row r="36" spans="2:65">
+    <row r="36" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
@@ -22511,7 +22459,7 @@
       </c>
       <c r="BM36"/>
     </row>
-    <row r="37" spans="2:65">
+    <row r="37" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
@@ -22665,7 +22613,7 @@
       </c>
       <c r="BM37"/>
     </row>
-    <row r="38" spans="2:65">
+    <row r="38" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
@@ -22819,7 +22767,7 @@
       </c>
       <c r="BM38"/>
     </row>
-    <row r="39" spans="2:65">
+    <row r="39" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
@@ -22973,7 +22921,7 @@
       </c>
       <c r="BM39"/>
     </row>
-    <row r="40" spans="2:65">
+    <row r="40" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
@@ -23050,7 +22998,7 @@
       <c r="BF40"/>
       <c r="BJ40"/>
     </row>
-    <row r="41" spans="2:65">
+    <row r="41" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
@@ -23081,7 +23029,7 @@
       <c r="BC41"/>
       <c r="BD41"/>
     </row>
-    <row r="42" spans="2:65">
+    <row r="42" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42"/>
@@ -23114,7 +23062,7 @@
       <c r="BB42"/>
       <c r="BD42"/>
     </row>
-    <row r="43" spans="2:65">
+    <row r="43" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B43"/>
       <c r="C43"/>
       <c r="D43"/>
@@ -23155,7 +23103,7 @@
       <c r="BF43"/>
       <c r="BG43"/>
     </row>
-    <row r="44" spans="2:65">
+    <row r="44" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
@@ -23196,7 +23144,7 @@
       <c r="BF44"/>
       <c r="BG44"/>
     </row>
-    <row r="45" spans="2:65">
+    <row r="45" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B45"/>
       <c r="C45"/>
       <c r="D45"/>
@@ -23237,7 +23185,7 @@
       <c r="BF45"/>
       <c r="BG45"/>
     </row>
-    <row r="46" spans="2:65">
+    <row r="46" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
@@ -23264,7 +23212,7 @@
       <c r="BF46"/>
       <c r="BG46"/>
     </row>
-    <row r="47" spans="2:65">
+    <row r="47" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B47"/>
       <c r="C47"/>
       <c r="D47"/>
@@ -23280,7 +23228,7 @@
       <c r="AF47"/>
       <c r="AI47"/>
     </row>
-    <row r="48" spans="2:65">
+    <row r="48" spans="2:65" x14ac:dyDescent="0.35">
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
@@ -23296,7 +23244,7 @@
       <c r="AF48"/>
       <c r="AI48"/>
     </row>
-    <row r="49" spans="2:37">
+    <row r="49" spans="2:37" x14ac:dyDescent="0.35">
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
@@ -23312,7 +23260,7 @@
       <c r="AF49"/>
       <c r="AI49"/>
     </row>
-    <row r="50" spans="2:37">
+    <row r="50" spans="2:37" x14ac:dyDescent="0.35">
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50"/>
@@ -23328,7 +23276,7 @@
       <c r="AF50"/>
       <c r="AI50"/>
     </row>
-    <row r="51" spans="2:37">
+    <row r="51" spans="2:37" x14ac:dyDescent="0.35">
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
@@ -23346,7 +23294,7 @@
       <c r="AJ51"/>
       <c r="AK51"/>
     </row>
-    <row r="52" spans="2:37">
+    <row r="52" spans="2:37" x14ac:dyDescent="0.35">
       <c r="W52"/>
       <c r="X52"/>
       <c r="Y52"/>
@@ -23361,7 +23309,7 @@
       <c r="AJ52"/>
       <c r="AK52"/>
     </row>
-    <row r="53" spans="2:37">
+    <row r="53" spans="2:37" x14ac:dyDescent="0.35">
       <c r="W53"/>
       <c r="X53"/>
       <c r="Y53"/>
@@ -23413,7 +23361,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="26" width="5.6328125" style="13" customWidth="1"/>
     <col min="27" max="27" width="20.6328125" style="13" customWidth="1"/>
@@ -23421,9 +23369,9 @@
     <col min="47" max="16384" width="8.90625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="12" customFormat="1" ht="26">
+    <row r="1" spans="1:39" s="12" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="10"/>
@@ -23449,7 +23397,7 @@
       <c r="W1" s="10"/>
       <c r="X1" s="10"/>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -23468,7 +23416,7 @@
       <c r="AG3"/>
       <c r="AH3"/>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -23485,7 +23433,7 @@
       <c r="AL4" s="15"/>
       <c r="AM4" s="15"/>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -23501,7 +23449,7 @@
       <c r="AI5" s="15"/>
       <c r="AJ5" s="15"/>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -23517,7 +23465,7 @@
       <c r="AI6" s="15"/>
       <c r="AJ6" s="15"/>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -23531,7 +23479,7 @@
       <c r="AG7"/>
       <c r="AH7"/>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -23545,7 +23493,7 @@
       <c r="AG8"/>
       <c r="AH8"/>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -23559,7 +23507,7 @@
       <c r="AG9"/>
       <c r="AH9"/>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -23577,7 +23525,7 @@
       <c r="AG10"/>
       <c r="AH10"/>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -23596,7 +23544,7 @@
       <c r="AG11"/>
       <c r="AH11"/>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -23615,7 +23563,7 @@
       <c r="AG12"/>
       <c r="AH12"/>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -23634,25 +23582,25 @@
       <c r="AG13" s="15"/>
       <c r="AH13" s="15"/>
     </row>
-    <row r="26" spans="2:40">
+    <row r="26" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="M26" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
-      <c r="Q26" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="R26" s="49"/>
-      <c r="S26" s="49"/>
+      <c r="I26" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="48"/>
+      <c r="K26" s="48"/>
+      <c r="M26" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="N26" s="48"/>
+      <c r="O26" s="48"/>
+      <c r="Q26" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="R26" s="48"/>
+      <c r="S26" s="48"/>
       <c r="U26" s="21"/>
       <c r="V26" s="21"/>
       <c r="W26" s="21"/>
@@ -23662,24 +23610,24 @@
       <c r="AA26" s="21"/>
       <c r="AB26" s="21"/>
       <c r="AC26" s="21"/>
-      <c r="AD26" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE26" s="46"/>
-      <c r="AF26" s="46"/>
+      <c r="AD26" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE26" s="45"/>
+      <c r="AF26" s="45"/>
       <c r="AG26" s="15"/>
-      <c r="AH26" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI26" s="46"/>
-      <c r="AJ26" s="46"/>
-      <c r="AL26" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="AM26" s="46"/>
-      <c r="AN26" s="46"/>
+      <c r="AH26" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI26" s="45"/>
+      <c r="AJ26" s="45"/>
+      <c r="AL26" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM26" s="45"/>
+      <c r="AN26" s="45"/>
     </row>
-    <row r="27" spans="2:40">
+    <row r="27" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B27" s="15"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
@@ -23702,7 +23650,7 @@
       <c r="AG27" s="15"/>
       <c r="AH27" s="15"/>
     </row>
-    <row r="28" spans="2:40">
+    <row r="28" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B28" s="39" t="s">
         <v>0</v>
       </c>
@@ -23710,13 +23658,13 @@
         <v>1</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F28" s="39" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G28" s="39" t="s">
         <v>10</v>
@@ -23767,7 +23715,7 @@
       </c>
       <c r="Z28" s="15"/>
       <c r="AA28" s="41" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AB28" s="41" t="s">
         <v>25</v>
@@ -23780,7 +23728,7 @@
         <v>14</v>
       </c>
       <c r="AF28" s="41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AH28" s="36" t="s">
         <v>1</v>
@@ -23789,7 +23737,7 @@
         <v>14</v>
       </c>
       <c r="AJ28" s="41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AL28" s="36" t="s">
         <v>1</v>
@@ -23798,10 +23746,10 @@
         <v>14</v>
       </c>
       <c r="AN28" s="41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="29" spans="2:40">
+    <row r="29" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B29" s="15"/>
       <c r="C29" s="15" t="s">
         <v>4</v>
@@ -23922,7 +23870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:40">
+    <row r="30" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B30" s="15"/>
       <c r="C30" s="15" t="s">
         <v>5</v>
@@ -24043,7 +23991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:40">
+    <row r="31" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B31" s="15"/>
       <c r="C31" s="15" t="s">
         <v>3</v>
@@ -24164,7 +24112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:40">
+    <row r="32" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B32" s="15"/>
       <c r="C32" s="15" t="s">
         <v>6</v>
@@ -24285,7 +24233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:40">
+    <row r="33" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B33" s="15"/>
       <c r="C33" s="15" t="s">
         <v>7</v>
@@ -24406,7 +24354,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:40">
+    <row r="34" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
@@ -24441,7 +24389,7 @@
       <c r="AG34" s="15"/>
       <c r="AH34" s="15"/>
     </row>
-    <row r="35" spans="2:40">
+    <row r="35" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
@@ -24473,7 +24421,7 @@
       <c r="AG35" s="26"/>
       <c r="AH35" s="26"/>
     </row>
-    <row r="36" spans="2:40">
+    <row r="36" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B36" s="24"/>
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
@@ -24500,7 +24448,7 @@
       <c r="AB36" s="14"/>
       <c r="AC36" s="14"/>
     </row>
-    <row r="37" spans="2:40">
+    <row r="37" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
       <c r="D37" s="14"/>

</xml_diff>